<commit_message>
Changed memory map Changed read configuration according memory map changes
</commit_message>
<xml_diff>
--- a/docs/EEPROM map.xlsx
+++ b/docs/EEPROM map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EEPROM Page 0" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="109">
   <si>
     <t>Main configuration page</t>
   </si>
@@ -455,23 +455,15 @@
 (S16) [mm]</t>
   </si>
   <si>
-    <t>Coxa 1/4 zero rotate
-(S16) [degree]</t>
-  </si>
-  <si>
-    <t>Coxa 2/5 zero rotate
-(S16) [degree]</t>
-  </si>
-  <si>
-    <t>Coxa 3/6 zero rotate
-(S16) [degree]</t>
-  </si>
-  <si>
     <t>Femur 1-6 zero rotate
 (S16) [degree]</t>
   </si>
   <si>
     <t>Tibia 1-6 zero rotate
+(S16) [degree]</t>
+  </si>
+  <si>
+    <t>Coxa 1 zero rotate
 (S16) [degree]</t>
   </si>
 </sst>
@@ -995,7 +987,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1106,23 +1098,68 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1139,59 +1176,22 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1567,7 +1567,7 @@
   </sheetPr>
   <dimension ref="B2:R21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2021,7 +2021,7 @@
   </sheetPr>
   <dimension ref="B2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2125,59 +2125,65 @@
       <c r="B6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65" t="s">
+      <c r="D6" s="40"/>
+      <c r="E6" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65" t="s">
+      <c r="F6" s="40"/>
+      <c r="G6" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="J6" s="65"/>
-      <c r="K6" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65" t="s">
-        <v>108</v>
-      </c>
-      <c r="N6" s="65"/>
-      <c r="O6" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="68" t="s">
-        <v>110</v>
-      </c>
-      <c r="R6" s="67"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="69"/>
+      <c r="Q6" s="69"/>
+      <c r="R6" s="70"/>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="26"/>
+      <c r="C7" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="N7" s="66"/>
+      <c r="O7" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="67" t="s">
+        <v>107</v>
+      </c>
+      <c r="R7" s="72"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
@@ -2473,567 +2479,563 @@
       </c>
       <c r="P21" s="39"/>
       <c r="Q21" s="39"/>
-      <c r="R21" s="40"/>
+      <c r="R21" s="46"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41">
+      <c r="C23" s="45"/>
+      <c r="D23" s="45">
         <v>7</v>
       </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41">
+      <c r="E23" s="45"/>
+      <c r="F23" s="45">
         <v>6</v>
       </c>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41">
+      <c r="G23" s="45"/>
+      <c r="H23" s="45">
         <v>5</v>
       </c>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41">
+      <c r="I23" s="45"/>
+      <c r="J23" s="45">
         <v>4</v>
       </c>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41">
+      <c r="K23" s="45"/>
+      <c r="L23" s="45">
         <v>3</v>
       </c>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41">
+      <c r="M23" s="45"/>
+      <c r="N23" s="45">
         <v>2</v>
       </c>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41">
+      <c r="O23" s="45"/>
+      <c r="P23" s="45">
         <v>1</v>
       </c>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="41">
+      <c r="Q23" s="45"/>
+      <c r="R23" s="45">
         <v>0</v>
       </c>
-      <c r="S23" s="41"/>
+      <c r="S23" s="45"/>
     </row>
     <row r="24" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="43" t="s">
+      <c r="C24" s="41"/>
+      <c r="D24" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="43"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="43"/>
-      <c r="R24" s="43"/>
-      <c r="S24" s="43"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="42"/>
+      <c r="S24" s="42"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="43"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="43"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="43"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="42"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="43"/>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="43"/>
-      <c r="R26" s="43"/>
-      <c r="S26" s="43"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="42"/>
+      <c r="Q26" s="42"/>
+      <c r="R26" s="42"/>
+      <c r="S26" s="42"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="43"/>
-      <c r="N27" s="43"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="43"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="42"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="42"/>
     </row>
     <row r="28" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45" t="s">
+      <c r="C28" s="43"/>
+      <c r="D28" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+      <c r="L28" s="44"/>
+      <c r="M28" s="44"/>
+      <c r="N28" s="44"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="44"/>
+      <c r="Q28" s="44"/>
+      <c r="R28" s="44"/>
+      <c r="S28" s="44"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="44"/>
+      <c r="P29" s="44"/>
+      <c r="Q29" s="44"/>
+      <c r="R29" s="44"/>
+      <c r="S29" s="44"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="45"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="44"/>
+      <c r="P30" s="44"/>
+      <c r="Q30" s="44"/>
+      <c r="R30" s="44"/>
+      <c r="S30" s="44"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="45"/>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
-      <c r="S31" s="45"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="44"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="44"/>
+      <c r="P31" s="44"/>
+      <c r="Q31" s="44"/>
+      <c r="R31" s="44"/>
+      <c r="S31" s="44"/>
     </row>
     <row r="32" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="42"/>
-      <c r="D32" s="43" t="s">
+      <c r="C32" s="41"/>
+      <c r="D32" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="43"/>
-      <c r="O32" s="43"/>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="43"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+      <c r="M32" s="42"/>
+      <c r="N32" s="42"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="42"/>
+      <c r="Q32" s="42"/>
+      <c r="R32" s="42"/>
+      <c r="S32" s="42"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="42"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="43"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="43"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="43"/>
-      <c r="P33" s="43"/>
-      <c r="Q33" s="43"/>
-      <c r="R33" s="43"/>
-      <c r="S33" s="43"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="42"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="42"/>
+      <c r="M33" s="42"/>
+      <c r="N33" s="42"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="42"/>
+      <c r="Q33" s="42"/>
+      <c r="R33" s="42"/>
+      <c r="S33" s="42"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="43"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="43"/>
-      <c r="P34" s="43"/>
-      <c r="Q34" s="43"/>
-      <c r="R34" s="43"/>
-      <c r="S34" s="43"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="42"/>
+      <c r="M34" s="42"/>
+      <c r="N34" s="42"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="42"/>
+      <c r="Q34" s="42"/>
+      <c r="R34" s="42"/>
+      <c r="S34" s="42"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="43"/>
-      <c r="R35" s="43"/>
-      <c r="S35" s="43"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="42"/>
+      <c r="M35" s="42"/>
+      <c r="N35" s="42"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="42"/>
+      <c r="Q35" s="42"/>
+      <c r="R35" s="42"/>
+      <c r="S35" s="42"/>
     </row>
     <row r="36" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="45" t="s">
+      <c r="C36" s="43"/>
+      <c r="D36" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="45"/>
-      <c r="R36" s="45"/>
-      <c r="S36" s="45"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
+      <c r="M36" s="44"/>
+      <c r="N36" s="44"/>
+      <c r="O36" s="44"/>
+      <c r="P36" s="44"/>
+      <c r="Q36" s="44"/>
+      <c r="R36" s="44"/>
+      <c r="S36" s="44"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="45"/>
-      <c r="R37" s="45"/>
-      <c r="S37" s="45"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+      <c r="L37" s="44"/>
+      <c r="M37" s="44"/>
+      <c r="N37" s="44"/>
+      <c r="O37" s="44"/>
+      <c r="P37" s="44"/>
+      <c r="Q37" s="44"/>
+      <c r="R37" s="44"/>
+      <c r="S37" s="44"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="45"/>
-      <c r="P38" s="45"/>
-      <c r="Q38" s="45"/>
-      <c r="R38" s="45"/>
-      <c r="S38" s="45"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44"/>
+      <c r="L38" s="44"/>
+      <c r="M38" s="44"/>
+      <c r="N38" s="44"/>
+      <c r="O38" s="44"/>
+      <c r="P38" s="44"/>
+      <c r="Q38" s="44"/>
+      <c r="R38" s="44"/>
+      <c r="S38" s="44"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
-      <c r="P39" s="45"/>
-      <c r="Q39" s="45"/>
-      <c r="R39" s="45"/>
-      <c r="S39" s="45"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+      <c r="L39" s="44"/>
+      <c r="M39" s="44"/>
+      <c r="N39" s="44"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="44"/>
+      <c r="Q39" s="44"/>
+      <c r="R39" s="44"/>
+      <c r="S39" s="44"/>
     </row>
     <row r="40" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="42"/>
-      <c r="D40" s="43" t="s">
+      <c r="C40" s="41"/>
+      <c r="D40" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="43"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="43"/>
-      <c r="M40" s="43"/>
-      <c r="N40" s="43"/>
-      <c r="O40" s="43"/>
-      <c r="P40" s="43"/>
-      <c r="Q40" s="43"/>
-      <c r="R40" s="43"/>
-      <c r="S40" s="43"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="42"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="42"/>
+      <c r="L40" s="42"/>
+      <c r="M40" s="42"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="42"/>
+      <c r="Q40" s="42"/>
+      <c r="R40" s="42"/>
+      <c r="S40" s="42"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43"/>
-      <c r="M41" s="43"/>
-      <c r="N41" s="43"/>
-      <c r="O41" s="43"/>
-      <c r="P41" s="43"/>
-      <c r="Q41" s="43"/>
-      <c r="R41" s="43"/>
-      <c r="S41" s="43"/>
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42"/>
+      <c r="K41" s="42"/>
+      <c r="L41" s="42"/>
+      <c r="M41" s="42"/>
+      <c r="N41" s="42"/>
+      <c r="O41" s="42"/>
+      <c r="P41" s="42"/>
+      <c r="Q41" s="42"/>
+      <c r="R41" s="42"/>
+      <c r="S41" s="42"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="43"/>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
-      <c r="K42" s="43"/>
-      <c r="L42" s="43"/>
-      <c r="M42" s="43"/>
-      <c r="N42" s="43"/>
-      <c r="O42" s="43"/>
-      <c r="P42" s="43"/>
-      <c r="Q42" s="43"/>
-      <c r="R42" s="43"/>
-      <c r="S42" s="43"/>
+      <c r="B42" s="41"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="42"/>
+      <c r="Q42" s="42"/>
+      <c r="R42" s="42"/>
+      <c r="S42" s="42"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B43" s="42"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="43"/>
-      <c r="H43" s="43"/>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="43"/>
-      <c r="M43" s="43"/>
-      <c r="N43" s="43"/>
-      <c r="O43" s="43"/>
-      <c r="P43" s="43"/>
-      <c r="Q43" s="43"/>
-      <c r="R43" s="43"/>
-      <c r="S43" s="43"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43" s="42"/>
+      <c r="I43" s="42"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="42"/>
+      <c r="L43" s="42"/>
+      <c r="M43" s="42"/>
+      <c r="N43" s="42"/>
+      <c r="O43" s="42"/>
+      <c r="P43" s="42"/>
+      <c r="Q43" s="42"/>
+      <c r="R43" s="42"/>
+      <c r="S43" s="42"/>
     </row>
     <row r="44" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="45" t="s">
+      <c r="C44" s="43"/>
+      <c r="D44" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="45"/>
-      <c r="M44" s="45"/>
-      <c r="N44" s="45"/>
-      <c r="O44" s="45"/>
-      <c r="P44" s="45"/>
-      <c r="Q44" s="45"/>
-      <c r="R44" s="45"/>
-      <c r="S44" s="45"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44"/>
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
+      <c r="M44" s="44"/>
+      <c r="N44" s="44"/>
+      <c r="O44" s="44"/>
+      <c r="P44" s="44"/>
+      <c r="Q44" s="44"/>
+      <c r="R44" s="44"/>
+      <c r="S44" s="44"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="45"/>
-      <c r="M45" s="45"/>
-      <c r="N45" s="45"/>
-      <c r="O45" s="45"/>
-      <c r="P45" s="45"/>
-      <c r="Q45" s="45"/>
-      <c r="R45" s="45"/>
-      <c r="S45" s="45"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="43"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
+      <c r="G45" s="44"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="44"/>
+      <c r="M45" s="44"/>
+      <c r="N45" s="44"/>
+      <c r="O45" s="44"/>
+      <c r="P45" s="44"/>
+      <c r="Q45" s="44"/>
+      <c r="R45" s="44"/>
+      <c r="S45" s="44"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="45"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="45"/>
-      <c r="M46" s="45"/>
-      <c r="N46" s="45"/>
-      <c r="O46" s="45"/>
-      <c r="P46" s="45"/>
-      <c r="Q46" s="45"/>
-      <c r="R46" s="45"/>
-      <c r="S46" s="45"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="44"/>
+      <c r="H46" s="44"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
+      <c r="K46" s="44"/>
+      <c r="L46" s="44"/>
+      <c r="M46" s="44"/>
+      <c r="N46" s="44"/>
+      <c r="O46" s="44"/>
+      <c r="P46" s="44"/>
+      <c r="Q46" s="44"/>
+      <c r="R46" s="44"/>
+      <c r="S46" s="44"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B47" s="44"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
-      <c r="M47" s="45"/>
-      <c r="N47" s="45"/>
-      <c r="O47" s="45"/>
-      <c r="P47" s="45"/>
-      <c r="Q47" s="45"/>
-      <c r="R47" s="45"/>
-      <c r="S47" s="45"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="44"/>
+      <c r="M47" s="44"/>
+      <c r="N47" s="44"/>
+      <c r="O47" s="44"/>
+      <c r="P47" s="44"/>
+      <c r="Q47" s="44"/>
+      <c r="R47" s="44"/>
+      <c r="S47" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="B40:C43"/>
-    <mergeCell ref="D40:S43"/>
-    <mergeCell ref="B44:C47"/>
-    <mergeCell ref="D44:S47"/>
-    <mergeCell ref="B28:C31"/>
-    <mergeCell ref="D28:S31"/>
-    <mergeCell ref="B32:C35"/>
-    <mergeCell ref="D32:S35"/>
-    <mergeCell ref="B36:C39"/>
-    <mergeCell ref="D36:S39"/>
+  <mergeCells count="34">
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="B2:R3"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
     <mergeCell ref="L23:M23"/>
     <mergeCell ref="N23:O23"/>
     <mergeCell ref="P23:Q23"/>
@@ -3045,11 +3047,18 @@
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="J23:K23"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="B2:R3"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B40:C43"/>
+    <mergeCell ref="D40:S43"/>
+    <mergeCell ref="B44:C47"/>
+    <mergeCell ref="D44:S47"/>
+    <mergeCell ref="B28:C31"/>
+    <mergeCell ref="D28:S31"/>
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="D32:S35"/>
+    <mergeCell ref="B36:C39"/>
+    <mergeCell ref="D36:S39"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3063,7 +3072,7 @@
   </sheetPr>
   <dimension ref="B2:V39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3173,36 +3182,36 @@
       <c r="D6" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47" t="s">
+      <c r="F6" s="61"/>
+      <c r="G6" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="47"/>
-      <c r="I6" s="46" t="s">
+      <c r="H6" s="62"/>
+      <c r="I6" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="46"/>
+      <c r="J6" s="61"/>
       <c r="K6" s="32" t="s">
         <v>61</v>
       </c>
       <c r="L6" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="M6" s="48" t="s">
+      <c r="M6" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="N6" s="48"/>
-      <c r="O6" s="49" t="s">
+      <c r="N6" s="63"/>
+      <c r="O6" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="48" t="s">
+      <c r="P6" s="64"/>
+      <c r="Q6" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="R6" s="50"/>
+      <c r="R6" s="65"/>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
@@ -3214,36 +3223,36 @@
       <c r="D7" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="54"/>
-      <c r="G7" s="55" t="s">
+      <c r="F7" s="58"/>
+      <c r="G7" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="55"/>
-      <c r="I7" s="54" t="s">
+      <c r="H7" s="59"/>
+      <c r="I7" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J7" s="54"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="28" t="s">
         <v>65</v>
       </c>
       <c r="L7" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="M7" s="51" t="s">
+      <c r="M7" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="N7" s="51"/>
-      <c r="O7" s="53" t="s">
+      <c r="N7" s="55"/>
+      <c r="O7" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="51" t="s">
+      <c r="P7" s="57"/>
+      <c r="Q7" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="R7" s="52"/>
+      <c r="R7" s="56"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
@@ -3255,36 +3264,36 @@
       <c r="D8" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="51"/>
-      <c r="G8" s="53" t="s">
+      <c r="F8" s="55"/>
+      <c r="G8" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="53"/>
-      <c r="I8" s="51" t="s">
+      <c r="H8" s="57"/>
+      <c r="I8" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="51"/>
+      <c r="J8" s="55"/>
       <c r="K8" s="29" t="s">
         <v>68</v>
       </c>
       <c r="L8" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="M8" s="54" t="s">
+      <c r="M8" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="N8" s="54"/>
-      <c r="O8" s="55" t="s">
+      <c r="N8" s="58"/>
+      <c r="O8" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="54" t="s">
+      <c r="P8" s="59"/>
+      <c r="Q8" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="R8" s="56"/>
+      <c r="R8" s="60"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
@@ -3296,36 +3305,36 @@
       <c r="D9" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="54"/>
-      <c r="G9" s="55" t="s">
+      <c r="F9" s="58"/>
+      <c r="G9" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="55"/>
-      <c r="I9" s="54" t="s">
+      <c r="H9" s="59"/>
+      <c r="I9" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="54"/>
+      <c r="J9" s="58"/>
       <c r="K9" s="28" t="s">
         <v>71</v>
       </c>
       <c r="L9" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="M9" s="51" t="s">
+      <c r="M9" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="N9" s="51"/>
-      <c r="O9" s="53" t="s">
+      <c r="N9" s="55"/>
+      <c r="O9" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="51" t="s">
+      <c r="P9" s="57"/>
+      <c r="Q9" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="R9" s="52"/>
+      <c r="R9" s="56"/>
     </row>
     <row r="10" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
@@ -3337,36 +3346,36 @@
       <c r="D10" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="51"/>
-      <c r="G10" s="53" t="s">
+      <c r="F10" s="55"/>
+      <c r="G10" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="51" t="s">
+      <c r="H10" s="57"/>
+      <c r="I10" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="51"/>
+      <c r="J10" s="55"/>
       <c r="K10" s="29" t="s">
         <v>74</v>
       </c>
       <c r="L10" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="M10" s="54" t="s">
+      <c r="M10" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="N10" s="54"/>
-      <c r="O10" s="55" t="s">
+      <c r="N10" s="58"/>
+      <c r="O10" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="54" t="s">
+      <c r="P10" s="59"/>
+      <c r="Q10" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="R10" s="56"/>
+      <c r="R10" s="60"/>
     </row>
     <row r="11" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
@@ -3378,36 +3387,36 @@
       <c r="D11" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="55" t="s">
+      <c r="F11" s="58"/>
+      <c r="G11" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="55"/>
-      <c r="I11" s="54" t="s">
+      <c r="H11" s="59"/>
+      <c r="I11" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="58"/>
       <c r="K11" s="28" t="s">
         <v>77</v>
       </c>
       <c r="L11" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="M11" s="51" t="s">
+      <c r="M11" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="N11" s="51"/>
-      <c r="O11" s="53" t="s">
+      <c r="N11" s="55"/>
+      <c r="O11" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="P11" s="53"/>
-      <c r="Q11" s="51" t="s">
+      <c r="P11" s="57"/>
+      <c r="Q11" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="R11" s="52"/>
+      <c r="R11" s="56"/>
     </row>
     <row r="12" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
@@ -3419,36 +3428,36 @@
       <c r="D12" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="51"/>
-      <c r="G12" s="53" t="s">
+      <c r="F12" s="55"/>
+      <c r="G12" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="53"/>
-      <c r="I12" s="51" t="s">
+      <c r="H12" s="57"/>
+      <c r="I12" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="J12" s="51"/>
+      <c r="J12" s="55"/>
       <c r="K12" s="29" t="s">
         <v>80</v>
       </c>
       <c r="L12" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="M12" s="54" t="s">
+      <c r="M12" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="N12" s="54"/>
-      <c r="O12" s="55" t="s">
+      <c r="N12" s="58"/>
+      <c r="O12" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="P12" s="55"/>
-      <c r="Q12" s="54" t="s">
+      <c r="P12" s="59"/>
+      <c r="Q12" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="R12" s="56"/>
+      <c r="R12" s="60"/>
     </row>
     <row r="13" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
@@ -3460,36 +3469,36 @@
       <c r="D13" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="54"/>
-      <c r="G13" s="55" t="s">
+      <c r="F13" s="58"/>
+      <c r="G13" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="55"/>
-      <c r="I13" s="54" t="s">
+      <c r="H13" s="59"/>
+      <c r="I13" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="J13" s="54"/>
+      <c r="J13" s="58"/>
       <c r="K13" s="28" t="s">
         <v>83</v>
       </c>
       <c r="L13" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="M13" s="51" t="s">
+      <c r="M13" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="N13" s="51"/>
-      <c r="O13" s="53" t="s">
+      <c r="N13" s="55"/>
+      <c r="O13" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="P13" s="53"/>
-      <c r="Q13" s="51" t="s">
+      <c r="P13" s="57"/>
+      <c r="Q13" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="R13" s="52"/>
+      <c r="R13" s="56"/>
     </row>
     <row r="14" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
@@ -3501,36 +3510,36 @@
       <c r="D14" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="51" t="s">
+      <c r="E14" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="51"/>
-      <c r="G14" s="53" t="s">
+      <c r="F14" s="55"/>
+      <c r="G14" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="53"/>
-      <c r="I14" s="51" t="s">
+      <c r="H14" s="57"/>
+      <c r="I14" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="J14" s="51"/>
+      <c r="J14" s="55"/>
       <c r="K14" s="29" t="s">
         <v>102</v>
       </c>
       <c r="L14" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="M14" s="54" t="s">
+      <c r="M14" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="N14" s="54"/>
-      <c r="O14" s="55" t="s">
+      <c r="N14" s="58"/>
+      <c r="O14" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="P14" s="55"/>
-      <c r="Q14" s="54" t="s">
+      <c r="P14" s="59"/>
+      <c r="Q14" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="R14" s="56"/>
+      <c r="R14" s="60"/>
     </row>
     <row r="15" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
@@ -3685,395 +3694,460 @@
       </c>
       <c r="P21" s="39"/>
       <c r="Q21" s="39"/>
-      <c r="R21" s="40"/>
+      <c r="R21" s="46"/>
       <c r="T21" s="23"/>
       <c r="U21" s="23"/>
       <c r="V21" s="23"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41">
+      <c r="C23" s="45"/>
+      <c r="D23" s="45">
         <v>7</v>
       </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41">
+      <c r="E23" s="45"/>
+      <c r="F23" s="45">
         <v>6</v>
       </c>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41">
+      <c r="G23" s="45"/>
+      <c r="H23" s="45">
         <v>5</v>
       </c>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41">
+      <c r="I23" s="45"/>
+      <c r="J23" s="45">
         <v>4</v>
       </c>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41">
+      <c r="K23" s="45"/>
+      <c r="L23" s="45">
         <v>3</v>
       </c>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41">
+      <c r="M23" s="45"/>
+      <c r="N23" s="45">
         <v>2</v>
       </c>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41">
+      <c r="O23" s="45"/>
+      <c r="P23" s="45">
         <v>1</v>
       </c>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="41">
+      <c r="Q23" s="45"/>
+      <c r="R23" s="45">
         <v>0</v>
       </c>
-      <c r="S23" s="41"/>
+      <c r="S23" s="45"/>
     </row>
     <row r="24" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="59" t="s">
+      <c r="C24" s="53"/>
+      <c r="D24" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="63" t="s">
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="M24" s="63"/>
-      <c r="N24" s="63" t="s">
+      <c r="M24" s="54"/>
+      <c r="N24" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63" t="s">
+      <c r="O24" s="54"/>
+      <c r="P24" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="59" t="s">
+      <c r="Q24" s="54"/>
+      <c r="R24" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="S24" s="59"/>
+      <c r="S24" s="50"/>
     </row>
     <row r="25" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="62"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="63"/>
-      <c r="M25" s="63"/>
-      <c r="N25" s="63"/>
-      <c r="O25" s="63"/>
-      <c r="P25" s="63"/>
-      <c r="Q25" s="63"/>
-      <c r="R25" s="59"/>
-      <c r="S25" s="59"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
+      <c r="P25" s="54"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="50"/>
     </row>
     <row r="26" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="63"/>
-      <c r="M26" s="63"/>
-      <c r="N26" s="63"/>
-      <c r="O26" s="63"/>
-      <c r="P26" s="63"/>
-      <c r="Q26" s="63"/>
-      <c r="R26" s="59"/>
-      <c r="S26" s="59"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="54"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="50"/>
+      <c r="S26" s="50"/>
     </row>
     <row r="27" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="62"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="63"/>
-      <c r="M27" s="63"/>
-      <c r="N27" s="63"/>
-      <c r="O27" s="63"/>
-      <c r="P27" s="63"/>
-      <c r="Q27" s="63"/>
-      <c r="R27" s="59"/>
-      <c r="S27" s="59"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="54"/>
+      <c r="P27" s="54"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="50"/>
     </row>
     <row r="28" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="58" t="s">
+      <c r="C28" s="51"/>
+      <c r="D28" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="E28" s="58"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="58"/>
-      <c r="N28" s="58"/>
-      <c r="O28" s="58"/>
-      <c r="P28" s="58"/>
-      <c r="Q28" s="58"/>
-      <c r="R28" s="58"/>
-      <c r="S28" s="58"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="49"/>
     </row>
     <row r="29" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="58"/>
-      <c r="L29" s="58"/>
-      <c r="M29" s="58"/>
-      <c r="N29" s="58"/>
-      <c r="O29" s="58"/>
-      <c r="P29" s="58"/>
-      <c r="Q29" s="58"/>
-      <c r="R29" s="58"/>
-      <c r="S29" s="58"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="49"/>
+      <c r="Q29" s="49"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
     </row>
     <row r="30" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="58"/>
-      <c r="L30" s="58"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="58"/>
-      <c r="P30" s="58"/>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="58"/>
-      <c r="S30" s="58"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="49"/>
+      <c r="P30" s="49"/>
+      <c r="Q30" s="49"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="49"/>
     </row>
     <row r="31" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="58"/>
-      <c r="Q31" s="58"/>
-      <c r="R31" s="58"/>
-      <c r="S31" s="58"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49"/>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="49"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="49"/>
     </row>
     <row r="32" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="58" t="s">
+      <c r="C32" s="52"/>
+      <c r="D32" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="58"/>
-      <c r="Q32" s="58"/>
-      <c r="R32" s="58"/>
-      <c r="S32" s="58"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="49"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
     </row>
     <row r="33" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="58"/>
-      <c r="R33" s="58"/>
-      <c r="S33" s="58"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
     </row>
     <row r="34" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="58"/>
-      <c r="S34" s="58"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
     </row>
     <row r="35" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
-      <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
-      <c r="R35" s="58"/>
-      <c r="S35" s="58"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="49"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
     </row>
     <row r="36" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="58" t="s">
+      <c r="C36" s="48"/>
+      <c r="D36" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="58"/>
-      <c r="L36" s="58"/>
-      <c r="M36" s="58"/>
-      <c r="N36" s="58"/>
-      <c r="O36" s="58"/>
-      <c r="P36" s="58"/>
-      <c r="Q36" s="58"/>
-      <c r="R36" s="58"/>
-      <c r="S36" s="58"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49"/>
+      <c r="N36" s="49"/>
+      <c r="O36" s="49"/>
+      <c r="P36" s="49"/>
+      <c r="Q36" s="49"/>
+      <c r="R36" s="49"/>
+      <c r="S36" s="49"/>
     </row>
     <row r="37" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="58"/>
-      <c r="L37" s="58"/>
-      <c r="M37" s="58"/>
-      <c r="N37" s="58"/>
-      <c r="O37" s="58"/>
-      <c r="P37" s="58"/>
-      <c r="Q37" s="58"/>
-      <c r="R37" s="58"/>
-      <c r="S37" s="58"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="49"/>
+      <c r="P37" s="49"/>
+      <c r="Q37" s="49"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="49"/>
     </row>
     <row r="38" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="58"/>
-      <c r="L38" s="58"/>
-      <c r="M38" s="58"/>
-      <c r="N38" s="58"/>
-      <c r="O38" s="58"/>
-      <c r="P38" s="58"/>
-      <c r="Q38" s="58"/>
-      <c r="R38" s="58"/>
-      <c r="S38" s="58"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="49"/>
+      <c r="O38" s="49"/>
+      <c r="P38" s="49"/>
+      <c r="Q38" s="49"/>
+      <c r="R38" s="49"/>
+      <c r="S38" s="49"/>
     </row>
     <row r="39" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="57"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="58"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
-      <c r="J39" s="58"/>
-      <c r="K39" s="58"/>
-      <c r="L39" s="58"/>
-      <c r="M39" s="58"/>
-      <c r="N39" s="58"/>
-      <c r="O39" s="58"/>
-      <c r="P39" s="58"/>
-      <c r="Q39" s="58"/>
-      <c r="R39" s="58"/>
-      <c r="S39" s="58"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="49"/>
+      <c r="O39" s="49"/>
+      <c r="P39" s="49"/>
+      <c r="Q39" s="49"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="77">
+    <mergeCell ref="B2:R3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
     <mergeCell ref="B36:C39"/>
     <mergeCell ref="D36:S39"/>
     <mergeCell ref="R24:S27"/>
@@ -4086,71 +4160,6 @@
     <mergeCell ref="L24:M27"/>
     <mergeCell ref="N24:O27"/>
     <mergeCell ref="P24:Q27"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="B2:R3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
FW: Added check coxa, femur and tibia angles (protection) Changed servo driver configuration Changed sequences Changed memory map Removed buzzer beep from error indication
SW:
Fixed module status update
</commit_message>
<xml_diff>
--- a/docs/EEPROM map.xlsx
+++ b/docs/EEPROM map.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EEPROM Page 0" sheetId="1" r:id="rId1"/>
     <sheet name="EEPROM Page 1" sheetId="2" r:id="rId2"/>
     <sheet name="EEPROM Page 2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="144525" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="113">
   <si>
     <t>Main configuration page</t>
   </si>
@@ -199,18 +199,6 @@
   <si>
     <t>Servo 0
 config</t>
-  </si>
-  <si>
-    <t>Logic zero
-(U16) [degree]</t>
-  </si>
-  <si>
-    <t>Protection min physic angle
-(U16) [degree]</t>
-  </si>
-  <si>
-    <t>Protection max physic angle
-(U16) [degree]</t>
   </si>
   <si>
     <t>Servo 1
@@ -466,12 +454,40 @@
     <t>Coxa 1 zero rotate
 (S16) [degree]</t>
   </si>
+  <si>
+    <t>Zero trim
+(S16) [degree]</t>
+  </si>
+  <si>
+    <t>(Protection) Coxa min angle
+(S16) [degree]</t>
+  </si>
+  <si>
+    <t>(Protection) Coxa max angle
+(S16) [degree]</t>
+  </si>
+  <si>
+    <t>(Protection) Femur min angle
+(S16) [degree]</t>
+  </si>
+  <si>
+    <t>(Protection) Femur max angle
+(S16) [degree]</t>
+  </si>
+  <si>
+    <t>(Protection) Tibia min angle
+(S16) [degree]</t>
+  </si>
+  <si>
+    <t>(Protection) Tibia max angle
+(S16) [degree]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -564,8 +580,16 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,6 +632,12 @@
         <bgColor rgb="FFC3D69B"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -987,7 +1017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1068,39 +1098,56 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1113,13 +1160,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1143,55 +1202,23 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1567,7 +1594,7 @@
   </sheetPr>
   <dimension ref="B2:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1576,44 +1603,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
     </row>
     <row r="5" spans="2:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
@@ -1997,12 +2024,12 @@
       <c r="L21" s="14"/>
       <c r="M21" s="14"/>
       <c r="N21" s="14"/>
-      <c r="O21" s="39" t="s">
+      <c r="O21" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2021,7 +2048,7 @@
   </sheetPr>
   <dimension ref="B2:S47"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2030,44 +2057,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2125,65 +2152,65 @@
       <c r="B6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="H6" s="40"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="70"/>
+      <c r="C6" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" s="44"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="39"/>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="71" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="N7" s="66"/>
-      <c r="O7" s="67" t="s">
-        <v>106</v>
-      </c>
-      <c r="P7" s="68"/>
-      <c r="Q7" s="67" t="s">
-        <v>107</v>
-      </c>
-      <c r="R7" s="72"/>
+      <c r="C7" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="N7" s="46"/>
+      <c r="O7" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="R7" s="54"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
@@ -2252,18 +2279,30 @@
       <c r="B11" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
+      <c r="C11" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="N11" s="71"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
@@ -2474,557 +2513,581 @@
       <c r="L21" s="14"/>
       <c r="M21" s="14"/>
       <c r="N21" s="14"/>
-      <c r="O21" s="39" t="s">
+      <c r="O21" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="46"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="42"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45">
+      <c r="C23" s="47"/>
+      <c r="D23" s="47">
         <v>7</v>
       </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45">
+      <c r="E23" s="47"/>
+      <c r="F23" s="47">
         <v>6</v>
       </c>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45">
+      <c r="G23" s="47"/>
+      <c r="H23" s="47">
         <v>5</v>
       </c>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45">
+      <c r="I23" s="47"/>
+      <c r="J23" s="47">
         <v>4</v>
       </c>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45">
+      <c r="K23" s="47"/>
+      <c r="L23" s="47">
         <v>3</v>
       </c>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45">
+      <c r="M23" s="47"/>
+      <c r="N23" s="47">
         <v>2</v>
       </c>
-      <c r="O23" s="45"/>
-      <c r="P23" s="45">
+      <c r="O23" s="47"/>
+      <c r="P23" s="47">
         <v>1</v>
       </c>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="45">
+      <c r="Q23" s="47"/>
+      <c r="R23" s="47">
         <v>0</v>
       </c>
-      <c r="S23" s="45"/>
+      <c r="S23" s="47"/>
     </row>
     <row r="24" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42" t="s">
+      <c r="C24" s="48"/>
+      <c r="D24" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
-      <c r="S24" s="42"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="42"/>
-      <c r="S25" s="42"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="49"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="49"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
-      <c r="S26" s="42"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="49"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="49"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="49"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="42"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="49"/>
+      <c r="O27" s="49"/>
+      <c r="P27" s="49"/>
+      <c r="Q27" s="49"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="49"/>
     </row>
     <row r="28" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="44" t="s">
+      <c r="C28" s="50"/>
+      <c r="D28" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="44"/>
-      <c r="F28" s="44"/>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
-      <c r="N28" s="44"/>
-      <c r="O28" s="44"/>
-      <c r="P28" s="44"/>
-      <c r="Q28" s="44"/>
-      <c r="R28" s="44"/>
-      <c r="S28" s="44"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="51"/>
+      <c r="R28" s="51"/>
+      <c r="S28" s="51"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="44"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="44"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="44"/>
-      <c r="P29" s="44"/>
-      <c r="Q29" s="44"/>
-      <c r="R29" s="44"/>
-      <c r="S29" s="44"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="51"/>
+      <c r="N29" s="51"/>
+      <c r="O29" s="51"/>
+      <c r="P29" s="51"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="51"/>
+      <c r="S29" s="51"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="44"/>
-      <c r="O30" s="44"/>
-      <c r="P30" s="44"/>
-      <c r="Q30" s="44"/>
-      <c r="R30" s="44"/>
-      <c r="S30" s="44"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="51"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="44"/>
-      <c r="P31" s="44"/>
-      <c r="Q31" s="44"/>
-      <c r="R31" s="44"/>
-      <c r="S31" s="44"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="51"/>
+      <c r="O31" s="51"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="51"/>
+      <c r="R31" s="51"/>
+      <c r="S31" s="51"/>
     </row>
     <row r="32" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="42" t="s">
+      <c r="C32" s="48"/>
+      <c r="D32" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="42"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="42"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="49"/>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="49"/>
+      <c r="R32" s="49"/>
+      <c r="S32" s="49"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="42"/>
-      <c r="L33" s="42"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="42"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="42"/>
-      <c r="Q33" s="42"/>
-      <c r="R33" s="42"/>
-      <c r="S33" s="42"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="49"/>
+      <c r="O33" s="49"/>
+      <c r="P33" s="49"/>
+      <c r="Q33" s="49"/>
+      <c r="R33" s="49"/>
+      <c r="S33" s="49"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="42"/>
-      <c r="Q34" s="42"/>
-      <c r="R34" s="42"/>
-      <c r="S34" s="42"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42"/>
-      <c r="K35" s="42"/>
-      <c r="L35" s="42"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="42"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="42"/>
-      <c r="Q35" s="42"/>
-      <c r="R35" s="42"/>
-      <c r="S35" s="42"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="49"/>
+      <c r="Q35" s="49"/>
+      <c r="R35" s="49"/>
+      <c r="S35" s="49"/>
     </row>
     <row r="36" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="43"/>
-      <c r="D36" s="44" t="s">
+      <c r="C36" s="50"/>
+      <c r="D36" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="44"/>
-      <c r="N36" s="44"/>
-      <c r="O36" s="44"/>
-      <c r="P36" s="44"/>
-      <c r="Q36" s="44"/>
-      <c r="R36" s="44"/>
-      <c r="S36" s="44"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="51"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="51"/>
+      <c r="O36" s="51"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="51"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="51"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="44"/>
-      <c r="L37" s="44"/>
-      <c r="M37" s="44"/>
-      <c r="N37" s="44"/>
-      <c r="O37" s="44"/>
-      <c r="P37" s="44"/>
-      <c r="Q37" s="44"/>
-      <c r="R37" s="44"/>
-      <c r="S37" s="44"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="51"/>
+      <c r="O37" s="51"/>
+      <c r="P37" s="51"/>
+      <c r="Q37" s="51"/>
+      <c r="R37" s="51"/>
+      <c r="S37" s="51"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="44"/>
-      <c r="L38" s="44"/>
-      <c r="M38" s="44"/>
-      <c r="N38" s="44"/>
-      <c r="O38" s="44"/>
-      <c r="P38" s="44"/>
-      <c r="Q38" s="44"/>
-      <c r="R38" s="44"/>
-      <c r="S38" s="44"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="51"/>
+      <c r="L38" s="51"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="51"/>
+      <c r="O38" s="51"/>
+      <c r="P38" s="51"/>
+      <c r="Q38" s="51"/>
+      <c r="R38" s="51"/>
+      <c r="S38" s="51"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="44"/>
-      <c r="L39" s="44"/>
-      <c r="M39" s="44"/>
-      <c r="N39" s="44"/>
-      <c r="O39" s="44"/>
-      <c r="P39" s="44"/>
-      <c r="Q39" s="44"/>
-      <c r="R39" s="44"/>
-      <c r="S39" s="44"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="51"/>
+      <c r="S39" s="51"/>
     </row>
     <row r="40" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="42" t="s">
+      <c r="C40" s="48"/>
+      <c r="D40" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="42"/>
-      <c r="J40" s="42"/>
-      <c r="K40" s="42"/>
-      <c r="L40" s="42"/>
-      <c r="M40" s="42"/>
-      <c r="N40" s="42"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="42"/>
-      <c r="Q40" s="42"/>
-      <c r="R40" s="42"/>
-      <c r="S40" s="42"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="Q40" s="49"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="49"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
-      <c r="K41" s="42"/>
-      <c r="L41" s="42"/>
-      <c r="M41" s="42"/>
-      <c r="N41" s="42"/>
-      <c r="O41" s="42"/>
-      <c r="P41" s="42"/>
-      <c r="Q41" s="42"/>
-      <c r="R41" s="42"/>
-      <c r="S41" s="42"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="49"/>
+      <c r="Q41" s="49"/>
+      <c r="R41" s="49"/>
+      <c r="S41" s="49"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="42"/>
-      <c r="L42" s="42"/>
-      <c r="M42" s="42"/>
-      <c r="N42" s="42"/>
-      <c r="O42" s="42"/>
-      <c r="P42" s="42"/>
-      <c r="Q42" s="42"/>
-      <c r="R42" s="42"/>
-      <c r="S42" s="42"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49"/>
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="49"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="42"/>
-      <c r="L43" s="42"/>
-      <c r="M43" s="42"/>
-      <c r="N43" s="42"/>
-      <c r="O43" s="42"/>
-      <c r="P43" s="42"/>
-      <c r="Q43" s="42"/>
-      <c r="R43" s="42"/>
-      <c r="S43" s="42"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="49"/>
+      <c r="O43" s="49"/>
+      <c r="P43" s="49"/>
+      <c r="Q43" s="49"/>
+      <c r="R43" s="49"/>
+      <c r="S43" s="49"/>
     </row>
     <row r="44" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="44" t="s">
+      <c r="C44" s="50"/>
+      <c r="D44" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="44"/>
-      <c r="L44" s="44"/>
-      <c r="M44" s="44"/>
-      <c r="N44" s="44"/>
-      <c r="O44" s="44"/>
-      <c r="P44" s="44"/>
-      <c r="Q44" s="44"/>
-      <c r="R44" s="44"/>
-      <c r="S44" s="44"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="51"/>
+      <c r="M44" s="51"/>
+      <c r="N44" s="51"/>
+      <c r="O44" s="51"/>
+      <c r="P44" s="51"/>
+      <c r="Q44" s="51"/>
+      <c r="R44" s="51"/>
+      <c r="S44" s="51"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="44"/>
-      <c r="L45" s="44"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="44"/>
-      <c r="O45" s="44"/>
-      <c r="P45" s="44"/>
-      <c r="Q45" s="44"/>
-      <c r="R45" s="44"/>
-      <c r="S45" s="44"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="51"/>
+      <c r="M45" s="51"/>
+      <c r="N45" s="51"/>
+      <c r="O45" s="51"/>
+      <c r="P45" s="51"/>
+      <c r="Q45" s="51"/>
+      <c r="R45" s="51"/>
+      <c r="S45" s="51"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
-      <c r="K46" s="44"/>
-      <c r="L46" s="44"/>
-      <c r="M46" s="44"/>
-      <c r="N46" s="44"/>
-      <c r="O46" s="44"/>
-      <c r="P46" s="44"/>
-      <c r="Q46" s="44"/>
-      <c r="R46" s="44"/>
-      <c r="S46" s="44"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="51"/>
+      <c r="M46" s="51"/>
+      <c r="N46" s="51"/>
+      <c r="O46" s="51"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="51"/>
+      <c r="R46" s="51"/>
+      <c r="S46" s="51"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="44"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
-      <c r="K47" s="44"/>
-      <c r="L47" s="44"/>
-      <c r="M47" s="44"/>
-      <c r="N47" s="44"/>
-      <c r="O47" s="44"/>
-      <c r="P47" s="44"/>
-      <c r="Q47" s="44"/>
-      <c r="R47" s="44"/>
-      <c r="S47" s="44"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="51"/>
+      <c r="O47" s="51"/>
+      <c r="P47" s="51"/>
+      <c r="Q47" s="51"/>
+      <c r="R47" s="51"/>
+      <c r="S47" s="51"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="40">
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="B40:C43"/>
+    <mergeCell ref="D40:S43"/>
+    <mergeCell ref="B44:C47"/>
+    <mergeCell ref="D44:S47"/>
+    <mergeCell ref="B28:C31"/>
+    <mergeCell ref="D28:S31"/>
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="D32:S35"/>
+    <mergeCell ref="B36:C39"/>
+    <mergeCell ref="D36:S39"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="B24:C27"/>
+    <mergeCell ref="D24:S27"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
     <mergeCell ref="O21:R21"/>
     <mergeCell ref="B2:R3"/>
     <mergeCell ref="C6:D6"/>
@@ -3036,29 +3099,11 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="M7:N7"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="B24:C27"/>
-    <mergeCell ref="D24:S27"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="B40:C43"/>
-    <mergeCell ref="D40:S43"/>
-    <mergeCell ref="B44:C47"/>
-    <mergeCell ref="D44:S47"/>
-    <mergeCell ref="B28:C31"/>
-    <mergeCell ref="D28:S31"/>
-    <mergeCell ref="B32:C35"/>
-    <mergeCell ref="D32:S35"/>
-    <mergeCell ref="B36:C39"/>
-    <mergeCell ref="D36:S39"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3072,7 +3117,7 @@
   </sheetPr>
   <dimension ref="B2:V39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3081,44 +3126,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3176,374 +3221,374 @@
       <c r="B6" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="37" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="61" t="s">
+      <c r="D6" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="55"/>
+      <c r="G6" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="67"/>
+      <c r="K6" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="61"/>
-      <c r="G6" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="62"/>
-      <c r="I6" s="61" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="61"/>
-      <c r="K6" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="M6" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="N6" s="63"/>
-      <c r="O6" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="P6" s="64"/>
-      <c r="Q6" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="R6" s="65"/>
+      <c r="L6" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="M6" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="N6" s="56"/>
+      <c r="O6" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" s="67"/>
+      <c r="Q6" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="68"/>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="58"/>
+      <c r="G7" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="66"/>
+      <c r="K7" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="59"/>
-      <c r="I7" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="58"/>
-      <c r="K7" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="M7" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="N7" s="55"/>
-      <c r="O7" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="R7" s="56"/>
+      <c r="L7" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="M7" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="N7" s="57"/>
+      <c r="O7" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="69"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="55"/>
-      <c r="G8" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="57"/>
-      <c r="I8" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="55"/>
-      <c r="K8" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="L8" s="29" t="s">
-        <v>100</v>
+      <c r="C8" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="57"/>
+      <c r="G8" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="66"/>
+      <c r="K8" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="35" t="s">
+        <v>97</v>
       </c>
       <c r="M8" s="58" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="N8" s="58"/>
-      <c r="O8" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="P8" s="59"/>
-      <c r="Q8" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="R8" s="60"/>
+      <c r="O8" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="69"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>100</v>
+        <v>63</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>97</v>
       </c>
       <c r="E9" s="58" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="F9" s="58"/>
-      <c r="G9" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" s="59"/>
-      <c r="I9" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" s="58"/>
-      <c r="K9" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="L9" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="M9" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="N9" s="55"/>
-      <c r="O9" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="P9" s="57"/>
-      <c r="Q9" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="R9" s="56"/>
+      <c r="G9" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="66"/>
+      <c r="K9" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="M9" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="N9" s="57"/>
+      <c r="O9" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="R9" s="69"/>
     </row>
     <row r="10" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="55"/>
-      <c r="G10" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="57"/>
-      <c r="I10" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="J10" s="55"/>
-      <c r="K10" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="L10" s="29" t="s">
-        <v>100</v>
+        <v>66</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="57"/>
+      <c r="G10" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="66"/>
+      <c r="K10" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="35" t="s">
+        <v>97</v>
       </c>
       <c r="M10" s="58" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="N10" s="58"/>
-      <c r="O10" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="R10" s="60"/>
+      <c r="O10" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="R10" s="69"/>
     </row>
     <row r="11" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>100</v>
+        <v>69</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>97</v>
       </c>
       <c r="E11" s="58" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="F11" s="58"/>
-      <c r="G11" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" s="58"/>
-      <c r="K11" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="L11" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="M11" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="N11" s="55"/>
-      <c r="O11" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="R11" s="56"/>
+      <c r="G11" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="66"/>
+      <c r="K11" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="L11" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="M11" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="N11" s="57"/>
+      <c r="O11" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" s="69"/>
     </row>
     <row r="12" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="55"/>
-      <c r="G12" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="57"/>
-      <c r="I12" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" s="55"/>
-      <c r="K12" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="L12" s="29" t="s">
-        <v>100</v>
+        <v>72</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="57"/>
+      <c r="G12" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="66"/>
+      <c r="K12" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" s="35" t="s">
+        <v>97</v>
       </c>
       <c r="M12" s="58" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="N12" s="58"/>
-      <c r="O12" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="R12" s="60"/>
+      <c r="O12" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="R12" s="69"/>
     </row>
     <row r="13" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>100</v>
+        <v>75</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>97</v>
       </c>
       <c r="E13" s="58" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="F13" s="58"/>
-      <c r="G13" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="59"/>
-      <c r="I13" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="J13" s="58"/>
-      <c r="K13" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="L13" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="M13" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="N13" s="55"/>
-      <c r="O13" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="P13" s="57"/>
-      <c r="Q13" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="R13" s="56"/>
+      <c r="G13" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="66"/>
+      <c r="K13" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="L13" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="M13" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="N13" s="57"/>
+      <c r="O13" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" s="69"/>
     </row>
     <row r="14" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="55"/>
-      <c r="G14" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="H14" s="57"/>
-      <c r="I14" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="55"/>
-      <c r="K14" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="L14" s="29" t="s">
-        <v>100</v>
+        <v>78</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="57"/>
+      <c r="G14" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="66"/>
+      <c r="K14" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="L14" s="35" t="s">
+        <v>97</v>
       </c>
       <c r="M14" s="58" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="N14" s="58"/>
-      <c r="O14" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="P14" s="59"/>
-      <c r="Q14" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="R14" s="60"/>
+      <c r="O14" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" s="69"/>
     </row>
     <row r="15" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="7"/>
@@ -3564,7 +3609,7 @@
     </row>
     <row r="16" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="7"/>
@@ -3585,7 +3630,7 @@
     </row>
     <row r="17" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="7"/>
@@ -3606,12 +3651,12 @@
     </row>
     <row r="18" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
+        <v>84</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="8"/>
@@ -3627,7 +3672,7 @@
     </row>
     <row r="19" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="22" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="7"/>
@@ -3651,7 +3696,7 @@
     </row>
     <row r="20" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="7"/>
@@ -3675,421 +3720,472 @@
     </row>
     <row r="21" spans="2:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C21" s="27"/>
-      <c r="D21" s="36"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="36"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="14"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
       <c r="M21" s="14"/>
       <c r="N21" s="14"/>
-      <c r="O21" s="39" t="s">
+      <c r="O21" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="46"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="42"/>
       <c r="T21" s="23"/>
       <c r="U21" s="23"/>
       <c r="V21" s="23"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45">
+      <c r="C23" s="47"/>
+      <c r="D23" s="47">
         <v>7</v>
       </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45">
+      <c r="E23" s="47"/>
+      <c r="F23" s="47">
         <v>6</v>
       </c>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45">
+      <c r="G23" s="47"/>
+      <c r="H23" s="47">
         <v>5</v>
       </c>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45">
+      <c r="I23" s="47"/>
+      <c r="J23" s="47">
         <v>4</v>
       </c>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45">
+      <c r="K23" s="47"/>
+      <c r="L23" s="47">
         <v>3</v>
       </c>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45">
+      <c r="M23" s="47"/>
+      <c r="N23" s="47">
         <v>2</v>
       </c>
-      <c r="O23" s="45"/>
-      <c r="P23" s="45">
+      <c r="O23" s="47"/>
+      <c r="P23" s="47">
         <v>1</v>
       </c>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="45">
+      <c r="Q23" s="47"/>
+      <c r="R23" s="47">
         <v>0</v>
       </c>
-      <c r="S23" s="45"/>
+      <c r="S23" s="47"/>
     </row>
     <row r="24" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="64"/>
+      <c r="D24" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" s="65"/>
+      <c r="N24" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="O24" s="65"/>
+      <c r="P24" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q24" s="65"/>
+      <c r="R24" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="S24" s="61"/>
+    </row>
+    <row r="25" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="65"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="65"/>
+      <c r="Q25" s="65"/>
+      <c r="R25" s="61"/>
+      <c r="S25" s="61"/>
+    </row>
+    <row r="26" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="64"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="65"/>
+      <c r="M26" s="65"/>
+      <c r="N26" s="65"/>
+      <c r="O26" s="65"/>
+      <c r="P26" s="65"/>
+      <c r="Q26" s="65"/>
+      <c r="R26" s="61"/>
+      <c r="S26" s="61"/>
+    </row>
+    <row r="27" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="65"/>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="61"/>
+      <c r="S27" s="61"/>
+    </row>
+    <row r="28" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="53"/>
-      <c r="D24" s="50" t="s">
+      <c r="C28" s="62"/>
+      <c r="D28" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="50"/>
-      <c r="K24" s="50"/>
-      <c r="L24" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="M24" s="54"/>
-      <c r="N24" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="O24" s="54"/>
-      <c r="P24" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="50" t="s">
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="60"/>
+      <c r="R28" s="60"/>
+      <c r="S28" s="60"/>
+    </row>
+    <row r="29" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
+      <c r="P29" s="60"/>
+      <c r="Q29" s="60"/>
+      <c r="R29" s="60"/>
+      <c r="S29" s="60"/>
+    </row>
+    <row r="30" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="62"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="60"/>
+      <c r="S30" s="60"/>
+    </row>
+    <row r="31" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="62"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="60"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="60"/>
+      <c r="P31" s="60"/>
+      <c r="Q31" s="60"/>
+      <c r="R31" s="60"/>
+      <c r="S31" s="60"/>
+    </row>
+    <row r="32" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="S24" s="50"/>
-    </row>
-    <row r="25" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="50"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="54"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="50"/>
-      <c r="S25" s="50"/>
-    </row>
-    <row r="26" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="54"/>
-      <c r="N26" s="54"/>
-      <c r="O26" s="54"/>
-      <c r="P26" s="54"/>
-      <c r="Q26" s="54"/>
-      <c r="R26" s="50"/>
-      <c r="S26" s="50"/>
-    </row>
-    <row r="27" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="54"/>
-      <c r="N27" s="54"/>
-      <c r="O27" s="54"/>
-      <c r="P27" s="54"/>
-      <c r="Q27" s="54"/>
-      <c r="R27" s="50"/>
-      <c r="S27" s="50"/>
-    </row>
-    <row r="28" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="51" t="s">
+      <c r="C32" s="63"/>
+      <c r="D32" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="49" t="s">
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="60"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="60"/>
+      <c r="R32" s="60"/>
+      <c r="S32" s="60"/>
+    </row>
+    <row r="33" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="63"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="60"/>
+    </row>
+    <row r="34" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="60"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="60"/>
+      <c r="S34" s="60"/>
+    </row>
+    <row r="35" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="63"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="60"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="60"/>
+    </row>
+    <row r="36" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="49"/>
-    </row>
-    <row r="29" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="49"/>
-      <c r="S29" s="49"/>
-    </row>
-    <row r="30" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
-      <c r="S30" s="49"/>
-    </row>
-    <row r="31" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
-      <c r="S31" s="49"/>
-    </row>
-    <row r="32" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="52" t="s">
+      <c r="C36" s="59"/>
+      <c r="D36" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="49"/>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="49"/>
-      <c r="S32" s="49"/>
-    </row>
-    <row r="33" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="52"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="49"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
-      <c r="S33" s="49"/>
-    </row>
-    <row r="34" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="49"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="49"/>
-      <c r="O34" s="49"/>
-      <c r="P34" s="49"/>
-      <c r="Q34" s="49"/>
-      <c r="R34" s="49"/>
-      <c r="S34" s="49"/>
-    </row>
-    <row r="35" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="52"/>
-      <c r="C35" s="52"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="49"/>
-      <c r="O35" s="49"/>
-      <c r="P35" s="49"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="49"/>
-      <c r="S35" s="49"/>
-    </row>
-    <row r="36" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="48"/>
-      <c r="D36" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="49"/>
-      <c r="N36" s="49"/>
-      <c r="O36" s="49"/>
-      <c r="P36" s="49"/>
-      <c r="Q36" s="49"/>
-      <c r="R36" s="49"/>
-      <c r="S36" s="49"/>
+      <c r="E36" s="60"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="60"/>
+      <c r="J36" s="60"/>
+      <c r="K36" s="60"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="60"/>
     </row>
     <row r="37" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="49"/>
-      <c r="O37" s="49"/>
-      <c r="P37" s="49"/>
-      <c r="Q37" s="49"/>
-      <c r="R37" s="49"/>
-      <c r="S37" s="49"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="60"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="60"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="60"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="60"/>
+      <c r="R37" s="60"/>
+      <c r="S37" s="60"/>
     </row>
     <row r="38" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="48"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="49"/>
-      <c r="H38" s="49"/>
-      <c r="I38" s="49"/>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="49"/>
-      <c r="P38" s="49"/>
-      <c r="Q38" s="49"/>
-      <c r="R38" s="49"/>
-      <c r="S38" s="49"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="60"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="60"/>
+      <c r="R38" s="60"/>
+      <c r="S38" s="60"/>
     </row>
     <row r="39" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="49"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="49"/>
-      <c r="R39" s="49"/>
-      <c r="S39" s="49"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="60"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="60"/>
+      <c r="I39" s="60"/>
+      <c r="J39" s="60"/>
+      <c r="K39" s="60"/>
+      <c r="L39" s="60"/>
+      <c r="M39" s="60"/>
+      <c r="N39" s="60"/>
+      <c r="O39" s="60"/>
+      <c r="P39" s="60"/>
+      <c r="Q39" s="60"/>
+      <c r="R39" s="60"/>
+      <c r="S39" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="B2:R3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="B36:C39"/>
+    <mergeCell ref="D36:S39"/>
+    <mergeCell ref="R24:S27"/>
+    <mergeCell ref="B28:C31"/>
+    <mergeCell ref="D28:S31"/>
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="D32:S35"/>
+    <mergeCell ref="B24:C27"/>
+    <mergeCell ref="D24:K27"/>
+    <mergeCell ref="L24:M27"/>
+    <mergeCell ref="N24:O27"/>
+    <mergeCell ref="P24:Q27"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
@@ -4102,64 +4198,13 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="B36:C39"/>
-    <mergeCell ref="D36:S39"/>
-    <mergeCell ref="R24:S27"/>
-    <mergeCell ref="B28:C31"/>
-    <mergeCell ref="D28:S31"/>
-    <mergeCell ref="B32:C35"/>
-    <mergeCell ref="D32:S35"/>
-    <mergeCell ref="B24:C27"/>
-    <mergeCell ref="D24:K27"/>
-    <mergeCell ref="L24:M27"/>
-    <mergeCell ref="N24:O27"/>
-    <mergeCell ref="P24:Q27"/>
+    <mergeCell ref="B2:R3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated memory map variables description
</commit_message>
<xml_diff>
--- a/docs/EEPROM map.xlsx
+++ b/docs/EEPROM map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EEPROM Page 0" sheetId="1" r:id="rId1"/>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Checksum</t>
-  </si>
-  <si>
-    <t>Limbs configuration page</t>
   </si>
   <si>
     <t>0x0100</t>
@@ -352,42 +349,6 @@
       <t>0`b — прямое направление
 1`b — обратное направление</t>
     </r>
-  </si>
-  <si>
-    <t>Logic zero
-(градусы)</t>
-  </si>
-  <si>
-    <t>Значение физического угла сервопривода, в котором будет находиться логический ноль</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">Protection min
-physic angle
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(градусы)</t>
-    </r>
-  </si>
-  <si>
-    <t>Минимальное значение физического угла сервопривода</t>
   </si>
   <si>
     <r>
@@ -481,6 +442,22 @@
   <si>
     <t>(Protection) Tibia max angle
 (S16) [degree]</t>
+  </si>
+  <si>
+    <t>PWM channel</t>
+  </si>
+  <si>
+    <t>Канал PWM для сервопривода</t>
+  </si>
+  <si>
+    <t>Zero Trim
+(градусы)</t>
+  </si>
+  <si>
+    <t>Коррекция нуля сервопривода</t>
+  </si>
+  <si>
+    <t>Motion core configuration page</t>
   </si>
 </sst>
 </file>
@@ -1130,6 +1107,24 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1145,21 +1140,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1169,55 +1149,52 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1594,7 +1571,7 @@
   </sheetPr>
   <dimension ref="B2:R21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2048,7 +2025,7 @@
   </sheetPr>
   <dimension ref="B2:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2058,7 +2035,7 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="40" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
@@ -2150,20 +2127,20 @@
     </row>
     <row r="6" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44" t="s">
-        <v>102</v>
-      </c>
-      <c r="H6" s="44"/>
+        <v>24</v>
+      </c>
+      <c r="C6" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="50"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
       <c r="K6" s="38"/>
@@ -2177,44 +2154,44 @@
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="L7" s="46"/>
-      <c r="M7" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="N7" s="46"/>
-      <c r="O7" s="52" t="s">
-        <v>103</v>
-      </c>
-      <c r="P7" s="53"/>
-      <c r="Q7" s="52" t="s">
-        <v>104</v>
-      </c>
-      <c r="R7" s="54"/>
+        <v>29</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="N7" s="52"/>
+      <c r="O7" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="53" t="s">
+        <v>99</v>
+      </c>
+      <c r="R7" s="55"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="7"/>
@@ -2235,7 +2212,7 @@
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="7"/>
@@ -2256,7 +2233,7 @@
     </row>
     <row r="10" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="7"/>
@@ -2277,32 +2254,32 @@
     </row>
     <row r="11" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42" t="s">
+        <v>106</v>
+      </c>
+      <c r="L11" s="42"/>
+      <c r="M11" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71" t="s">
-        <v>110</v>
-      </c>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71" t="s">
-        <v>111</v>
-      </c>
-      <c r="L11" s="71"/>
-      <c r="M11" s="71" t="s">
-        <v>112</v>
-      </c>
-      <c r="N11" s="71"/>
+      <c r="N11" s="42"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
@@ -2310,7 +2287,7 @@
     </row>
     <row r="12" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="7"/>
@@ -2331,7 +2308,7 @@
     </row>
     <row r="13" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="7"/>
@@ -2352,7 +2329,7 @@
     </row>
     <row r="14" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="7"/>
@@ -2373,7 +2350,7 @@
     </row>
     <row r="15" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="7"/>
@@ -2394,7 +2371,7 @@
     </row>
     <row r="16" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="7"/>
@@ -2415,7 +2392,7 @@
     </row>
     <row r="17" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="7"/>
@@ -2436,7 +2413,7 @@
     </row>
     <row r="18" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="7"/>
@@ -2457,7 +2434,7 @@
     </row>
     <row r="19" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="7"/>
@@ -2478,7 +2455,7 @@
     </row>
     <row r="20" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="7"/>
@@ -2499,7 +2476,7 @@
     </row>
     <row r="21" spans="2:19" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="14"/>
@@ -2518,11 +2495,11 @@
       </c>
       <c r="P21" s="41"/>
       <c r="Q21" s="41"/>
-      <c r="R21" s="42"/>
+      <c r="R21" s="48"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B23" s="47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="47"/>
       <c r="D23" s="47">
@@ -2559,535 +2536,511 @@
       <c r="S23" s="47"/>
     </row>
     <row r="24" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="43"/>
+      <c r="D24" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49" t="s">
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="44"/>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="44"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="44"/>
+      <c r="Q25" s="44"/>
+      <c r="R25" s="44"/>
+      <c r="S25" s="44"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+    </row>
+    <row r="28" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="49"/>
-      <c r="Q24" s="49"/>
-      <c r="R24" s="49"/>
-      <c r="S24" s="49"/>
-    </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="49"/>
-      <c r="Q25" s="49"/>
-      <c r="R25" s="49"/>
-      <c r="S25" s="49"/>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="49"/>
-      <c r="Q26" s="49"/>
-      <c r="R26" s="49"/>
-      <c r="S26" s="49"/>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="49"/>
-      <c r="O27" s="49"/>
-      <c r="P27" s="49"/>
-      <c r="Q27" s="49"/>
-      <c r="R27" s="49"/>
-      <c r="S27" s="49"/>
-    </row>
-    <row r="28" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="50" t="s">
+      <c r="C28" s="45"/>
+      <c r="D28" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="51" t="s">
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="46"/>
+      <c r="P28" s="46"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="46"/>
+      <c r="S28" s="46"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="46"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
+      <c r="S29" s="46"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="46"/>
+      <c r="Q30" s="46"/>
+      <c r="R30" s="46"/>
+      <c r="S30" s="46"/>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="46"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="46"/>
+      <c r="O31" s="46"/>
+      <c r="P31" s="46"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="46"/>
+      <c r="S31" s="46"/>
+    </row>
+    <row r="32" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="51"/>
-    </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51"/>
-      <c r="O29" s="51"/>
-      <c r="P29" s="51"/>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="51"/>
-      <c r="S29" s="51"/>
-    </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="51"/>
-      <c r="M30" s="51"/>
-      <c r="N30" s="51"/>
-      <c r="O30" s="51"/>
-      <c r="P30" s="51"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="51"/>
-      <c r="S30" s="51"/>
-    </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="51"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="51"/>
-      <c r="O31" s="51"/>
-      <c r="P31" s="51"/>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="51"/>
-      <c r="S31" s="51"/>
-    </row>
-    <row r="32" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="48" t="s">
+      <c r="C32" s="43"/>
+      <c r="D32" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="49" t="s">
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="44"/>
+      <c r="M32" s="44"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="44"/>
+      <c r="P32" s="44"/>
+      <c r="Q32" s="44"/>
+      <c r="R32" s="44"/>
+      <c r="S32" s="44"/>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="44"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="44"/>
+      <c r="Q33" s="44"/>
+      <c r="R33" s="44"/>
+      <c r="S33" s="44"/>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="44"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="44"/>
+      <c r="Q34" s="44"/>
+      <c r="R34" s="44"/>
+      <c r="S34" s="44"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="44"/>
+      <c r="P35" s="44"/>
+      <c r="Q35" s="44"/>
+      <c r="R35" s="44"/>
+      <c r="S35" s="44"/>
+    </row>
+    <row r="36" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="45"/>
+      <c r="D36" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="49"/>
-      <c r="P32" s="49"/>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="49"/>
-      <c r="S32" s="49"/>
-    </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="49"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
-      <c r="S33" s="49"/>
-    </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="49"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="49"/>
-      <c r="O34" s="49"/>
-      <c r="P34" s="49"/>
-      <c r="Q34" s="49"/>
-      <c r="R34" s="49"/>
-      <c r="S34" s="49"/>
-    </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="49"/>
-      <c r="O35" s="49"/>
-      <c r="P35" s="49"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="49"/>
-      <c r="S35" s="49"/>
-    </row>
-    <row r="36" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="50" t="s">
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="46"/>
+      <c r="O36" s="46"/>
+      <c r="P36" s="46"/>
+      <c r="Q36" s="46"/>
+      <c r="R36" s="46"/>
+      <c r="S36" s="46"/>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="46"/>
+      <c r="N37" s="46"/>
+      <c r="O37" s="46"/>
+      <c r="P37" s="46"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="46"/>
+      <c r="S37" s="46"/>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="46"/>
+      <c r="O38" s="46"/>
+      <c r="P38" s="46"/>
+      <c r="Q38" s="46"/>
+      <c r="R38" s="46"/>
+      <c r="S38" s="46"/>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B39" s="45"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
+      <c r="N39" s="46"/>
+      <c r="O39" s="46"/>
+      <c r="P39" s="46"/>
+      <c r="Q39" s="46"/>
+      <c r="R39" s="46"/>
+      <c r="S39" s="46"/>
+    </row>
+    <row r="40" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="51" t="s">
+      <c r="C40" s="43"/>
+      <c r="D40" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="51"/>
-      <c r="M36" s="51"/>
-      <c r="N36" s="51"/>
-      <c r="O36" s="51"/>
-      <c r="P36" s="51"/>
-      <c r="Q36" s="51"/>
-      <c r="R36" s="51"/>
-      <c r="S36" s="51"/>
-    </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
-      <c r="I37" s="51"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="51"/>
-      <c r="L37" s="51"/>
-      <c r="M37" s="51"/>
-      <c r="N37" s="51"/>
-      <c r="O37" s="51"/>
-      <c r="P37" s="51"/>
-      <c r="Q37" s="51"/>
-      <c r="R37" s="51"/>
-      <c r="S37" s="51"/>
-    </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="51"/>
-      <c r="I38" s="51"/>
-      <c r="J38" s="51"/>
-      <c r="K38" s="51"/>
-      <c r="L38" s="51"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="51"/>
-      <c r="O38" s="51"/>
-      <c r="P38" s="51"/>
-      <c r="Q38" s="51"/>
-      <c r="R38" s="51"/>
-      <c r="S38" s="51"/>
-    </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="51"/>
-      <c r="O39" s="51"/>
-      <c r="P39" s="51"/>
-      <c r="Q39" s="51"/>
-      <c r="R39" s="51"/>
-      <c r="S39" s="51"/>
-    </row>
-    <row r="40" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="48" t="s">
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="44"/>
+      <c r="M40" s="44"/>
+      <c r="N40" s="44"/>
+      <c r="O40" s="44"/>
+      <c r="P40" s="44"/>
+      <c r="Q40" s="44"/>
+      <c r="R40" s="44"/>
+      <c r="S40" s="44"/>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="44"/>
+      <c r="M41" s="44"/>
+      <c r="N41" s="44"/>
+      <c r="O41" s="44"/>
+      <c r="P41" s="44"/>
+      <c r="Q41" s="44"/>
+      <c r="R41" s="44"/>
+      <c r="S41" s="44"/>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="44"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44"/>
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="44"/>
+      <c r="S42" s="44"/>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44"/>
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="44"/>
+      <c r="S43" s="44"/>
+    </row>
+    <row r="44" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="48"/>
-      <c r="D40" s="49" t="s">
+      <c r="C44" s="45"/>
+      <c r="D44" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="49"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="49"/>
-      <c r="H40" s="49"/>
-      <c r="I40" s="49"/>
-      <c r="J40" s="49"/>
-      <c r="K40" s="49"/>
-      <c r="L40" s="49"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="49"/>
-      <c r="O40" s="49"/>
-      <c r="P40" s="49"/>
-      <c r="Q40" s="49"/>
-      <c r="R40" s="49"/>
-      <c r="S40" s="49"/>
-    </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
-      <c r="H41" s="49"/>
-      <c r="I41" s="49"/>
-      <c r="J41" s="49"/>
-      <c r="K41" s="49"/>
-      <c r="L41" s="49"/>
-      <c r="M41" s="49"/>
-      <c r="N41" s="49"/>
-      <c r="O41" s="49"/>
-      <c r="P41" s="49"/>
-      <c r="Q41" s="49"/>
-      <c r="R41" s="49"/>
-      <c r="S41" s="49"/>
-    </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49"/>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49"/>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="49"/>
-      <c r="S42" s="49"/>
-    </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
-      <c r="K43" s="49"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="49"/>
-      <c r="O43" s="49"/>
-      <c r="P43" s="49"/>
-      <c r="Q43" s="49"/>
-      <c r="R43" s="49"/>
-      <c r="S43" s="49"/>
-    </row>
-    <row r="44" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C44" s="50"/>
-      <c r="D44" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="51"/>
-      <c r="I44" s="51"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="51"/>
-      <c r="O44" s="51"/>
-      <c r="P44" s="51"/>
-      <c r="Q44" s="51"/>
-      <c r="R44" s="51"/>
-      <c r="S44" s="51"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="46"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="46"/>
+      <c r="M44" s="46"/>
+      <c r="N44" s="46"/>
+      <c r="O44" s="46"/>
+      <c r="P44" s="46"/>
+      <c r="Q44" s="46"/>
+      <c r="R44" s="46"/>
+      <c r="S44" s="46"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="51"/>
-      <c r="I45" s="51"/>
-      <c r="J45" s="51"/>
-      <c r="K45" s="51"/>
-      <c r="L45" s="51"/>
-      <c r="M45" s="51"/>
-      <c r="N45" s="51"/>
-      <c r="O45" s="51"/>
-      <c r="P45" s="51"/>
-      <c r="Q45" s="51"/>
-      <c r="R45" s="51"/>
-      <c r="S45" s="51"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="46"/>
+      <c r="M45" s="46"/>
+      <c r="N45" s="46"/>
+      <c r="O45" s="46"/>
+      <c r="P45" s="46"/>
+      <c r="Q45" s="46"/>
+      <c r="R45" s="46"/>
+      <c r="S45" s="46"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="51"/>
-      <c r="I46" s="51"/>
-      <c r="J46" s="51"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="51"/>
-      <c r="M46" s="51"/>
-      <c r="N46" s="51"/>
-      <c r="O46" s="51"/>
-      <c r="P46" s="51"/>
-      <c r="Q46" s="51"/>
-      <c r="R46" s="51"/>
-      <c r="S46" s="51"/>
+      <c r="B46" s="45"/>
+      <c r="C46" s="45"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="46"/>
+      <c r="M46" s="46"/>
+      <c r="N46" s="46"/>
+      <c r="O46" s="46"/>
+      <c r="P46" s="46"/>
+      <c r="Q46" s="46"/>
+      <c r="R46" s="46"/>
+      <c r="S46" s="46"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="51"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="51"/>
-      <c r="H47" s="51"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="51"/>
-      <c r="K47" s="51"/>
-      <c r="L47" s="51"/>
-      <c r="M47" s="51"/>
-      <c r="N47" s="51"/>
-      <c r="O47" s="51"/>
-      <c r="P47" s="51"/>
-      <c r="Q47" s="51"/>
-      <c r="R47" s="51"/>
-      <c r="S47" s="51"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="46"/>
+      <c r="N47" s="46"/>
+      <c r="O47" s="46"/>
+      <c r="P47" s="46"/>
+      <c r="Q47" s="46"/>
+      <c r="R47" s="46"/>
+      <c r="S47" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="B40:C43"/>
-    <mergeCell ref="D40:S43"/>
-    <mergeCell ref="B44:C47"/>
-    <mergeCell ref="D44:S47"/>
-    <mergeCell ref="B28:C31"/>
-    <mergeCell ref="D28:S31"/>
-    <mergeCell ref="B32:C35"/>
-    <mergeCell ref="D32:S35"/>
-    <mergeCell ref="B36:C39"/>
-    <mergeCell ref="D36:S39"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="B24:C27"/>
-    <mergeCell ref="D24:S27"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
     <mergeCell ref="O21:R21"/>
     <mergeCell ref="B2:R3"/>
     <mergeCell ref="C6:D6"/>
@@ -3104,6 +3057,30 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B44:C47"/>
+    <mergeCell ref="D44:S47"/>
+    <mergeCell ref="B28:C31"/>
+    <mergeCell ref="D28:S31"/>
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="D32:S35"/>
+    <mergeCell ref="B36:C39"/>
+    <mergeCell ref="D36:S39"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="B40:C43"/>
+    <mergeCell ref="D40:S43"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="B24:C27"/>
+    <mergeCell ref="D24:S27"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3127,7 +3104,7 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
@@ -3219,376 +3196,376 @@
     </row>
     <row r="6" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="D6" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="68"/>
+      <c r="G6" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="69"/>
+      <c r="K6" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" s="55"/>
-      <c r="G6" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="67"/>
-      <c r="K6" s="37" t="s">
-        <v>58</v>
-      </c>
       <c r="L6" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="M6" s="56" t="s">
-        <v>106</v>
-      </c>
-      <c r="N6" s="56"/>
-      <c r="O6" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="68"/>
+        <v>92</v>
+      </c>
+      <c r="M6" s="70" t="s">
+        <v>101</v>
+      </c>
+      <c r="N6" s="70"/>
+      <c r="O6" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="69"/>
+      <c r="Q6" s="69" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="71"/>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="67"/>
+      <c r="G7" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="64"/>
+      <c r="K7" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="66"/>
-      <c r="K7" s="34" t="s">
-        <v>62</v>
-      </c>
       <c r="L7" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="M7" s="57" t="s">
-        <v>106</v>
-      </c>
-      <c r="N7" s="57"/>
-      <c r="O7" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7" s="69"/>
+        <v>92</v>
+      </c>
+      <c r="M7" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7" s="66"/>
+      <c r="O7" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="64"/>
+      <c r="Q7" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="65"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="66"/>
+      <c r="G8" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="64"/>
+      <c r="K8" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="57" t="s">
-        <v>106</v>
-      </c>
-      <c r="F8" s="57"/>
-      <c r="G8" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="66"/>
-      <c r="K8" s="35" t="s">
-        <v>65</v>
-      </c>
       <c r="L8" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="M8" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="N8" s="58"/>
-      <c r="O8" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="R8" s="69"/>
+        <v>92</v>
+      </c>
+      <c r="M8" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="N8" s="67"/>
+      <c r="O8" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="64"/>
+      <c r="Q8" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="65"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="67"/>
+      <c r="G9" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="64"/>
+      <c r="K9" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="66"/>
-      <c r="K9" s="34" t="s">
-        <v>68</v>
-      </c>
       <c r="L9" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="M9" s="57" t="s">
-        <v>106</v>
-      </c>
-      <c r="N9" s="57"/>
-      <c r="O9" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9" s="66"/>
-      <c r="Q9" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="R9" s="69"/>
+        <v>92</v>
+      </c>
+      <c r="M9" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="N9" s="66"/>
+      <c r="O9" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="64"/>
+      <c r="Q9" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="65"/>
     </row>
     <row r="10" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="66"/>
+      <c r="G10" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="64"/>
+      <c r="K10" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="66"/>
-      <c r="K10" s="35" t="s">
-        <v>71</v>
-      </c>
       <c r="L10" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="M10" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="N10" s="58"/>
-      <c r="O10" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="R10" s="69"/>
+        <v>92</v>
+      </c>
+      <c r="M10" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="N10" s="67"/>
+      <c r="O10" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="64"/>
+      <c r="Q10" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="65"/>
     </row>
     <row r="11" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="67"/>
+      <c r="G11" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="64"/>
+      <c r="K11" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="58"/>
-      <c r="G11" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="66"/>
-      <c r="I11" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="66"/>
-      <c r="K11" s="34" t="s">
-        <v>74</v>
-      </c>
       <c r="L11" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="M11" s="57" t="s">
-        <v>106</v>
-      </c>
-      <c r="N11" s="57"/>
-      <c r="O11" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="R11" s="69"/>
+        <v>92</v>
+      </c>
+      <c r="M11" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="N11" s="66"/>
+      <c r="O11" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" s="65"/>
     </row>
     <row r="12" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="66"/>
+      <c r="G12" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="64"/>
+      <c r="K12" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12" s="57" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="57"/>
-      <c r="G12" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="66"/>
-      <c r="K12" s="35" t="s">
-        <v>77</v>
-      </c>
       <c r="L12" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="M12" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="N12" s="58"/>
-      <c r="O12" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="R12" s="69"/>
+        <v>92</v>
+      </c>
+      <c r="M12" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="N12" s="67"/>
+      <c r="O12" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" s="65"/>
     </row>
     <row r="13" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="67"/>
+      <c r="G13" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="64"/>
+      <c r="K13" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13" s="58"/>
-      <c r="G13" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="66"/>
-      <c r="K13" s="34" t="s">
-        <v>80</v>
-      </c>
       <c r="L13" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="M13" s="57" t="s">
-        <v>106</v>
-      </c>
-      <c r="N13" s="57"/>
-      <c r="O13" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="P13" s="66"/>
-      <c r="Q13" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="R13" s="69"/>
+        <v>92</v>
+      </c>
+      <c r="M13" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="N13" s="66"/>
+      <c r="O13" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="64"/>
+      <c r="Q13" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" s="65"/>
     </row>
     <row r="14" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="57" t="s">
-        <v>106</v>
-      </c>
-      <c r="F14" s="57"/>
-      <c r="G14" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="66"/>
+        <v>92</v>
+      </c>
+      <c r="E14" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="66"/>
+      <c r="G14" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="64"/>
       <c r="K14" s="35" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L14" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="M14" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="N14" s="58"/>
-      <c r="O14" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="P14" s="66"/>
-      <c r="Q14" s="66" t="s">
-        <v>29</v>
-      </c>
-      <c r="R14" s="69"/>
+        <v>92</v>
+      </c>
+      <c r="M14" s="67" t="s">
+        <v>101</v>
+      </c>
+      <c r="N14" s="67"/>
+      <c r="O14" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="64"/>
+      <c r="Q14" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R14" s="65"/>
     </row>
     <row r="15" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="7"/>
@@ -3609,7 +3586,7 @@
     </row>
     <row r="16" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="7"/>
@@ -3630,7 +3607,7 @@
     </row>
     <row r="17" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="7"/>
@@ -3651,7 +3628,7 @@
     </row>
     <row r="18" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="32"/>
       <c r="D18" s="28"/>
@@ -3672,7 +3649,7 @@
     </row>
     <row r="19" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="7"/>
@@ -3696,7 +3673,7 @@
     </row>
     <row r="20" spans="2:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="7"/>
@@ -3720,7 +3697,7 @@
     </row>
     <row r="21" spans="2:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="27"/>
       <c r="D21" s="33"/>
@@ -3739,14 +3716,14 @@
       </c>
       <c r="P21" s="41"/>
       <c r="Q21" s="41"/>
-      <c r="R21" s="42"/>
+      <c r="R21" s="48"/>
       <c r="T21" s="23"/>
       <c r="U21" s="23"/>
       <c r="V21" s="23"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B23" s="47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" s="47"/>
       <c r="D23" s="47">
@@ -3783,351 +3760,416 @@
       <c r="S23" s="47"/>
     </row>
     <row r="24" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="62"/>
+      <c r="D24" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="61" t="s">
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="63"/>
+      <c r="N24" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="63"/>
+      <c r="P24" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" s="63"/>
+      <c r="R24" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="M24" s="65"/>
-      <c r="N24" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="O24" s="65"/>
-      <c r="P24" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q24" s="65"/>
-      <c r="R24" s="61" t="s">
+      <c r="S24" s="59"/>
+    </row>
+    <row r="25" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="63"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="63"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+    </row>
+    <row r="26" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="63"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="63"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="63"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
+    </row>
+    <row r="27" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="62"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="59"/>
+      <c r="S27" s="59"/>
+    </row>
+    <row r="28" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="60"/>
+      <c r="D28" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="58"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="58"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="58"/>
+      <c r="R28" s="58"/>
+      <c r="S28" s="58"/>
+    </row>
+    <row r="29" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="58"/>
+      <c r="I29" s="58"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="58"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="58"/>
+      <c r="P29" s="58"/>
+      <c r="Q29" s="58"/>
+      <c r="R29" s="58"/>
+      <c r="S29" s="58"/>
+    </row>
+    <row r="30" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="58"/>
+      <c r="I30" s="58"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="58"/>
+      <c r="L30" s="58"/>
+      <c r="M30" s="58"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="58"/>
+      <c r="P30" s="58"/>
+      <c r="Q30" s="58"/>
+      <c r="R30" s="58"/>
+      <c r="S30" s="58"/>
+    </row>
+    <row r="31" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="58"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="58"/>
+    </row>
+    <row r="32" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="61"/>
+      <c r="D32" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="58"/>
+      <c r="N32" s="58"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="58"/>
+      <c r="Q32" s="58"/>
+      <c r="R32" s="58"/>
+      <c r="S32" s="58"/>
+    </row>
+    <row r="33" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="58"/>
+      <c r="R33" s="58"/>
+      <c r="S33" s="58"/>
+    </row>
+    <row r="34" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="61"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="58"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="58"/>
+      <c r="R34" s="58"/>
+      <c r="S34" s="58"/>
+    </row>
+    <row r="35" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="58"/>
+      <c r="J35" s="58"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="58"/>
+      <c r="M35" s="58"/>
+      <c r="N35" s="58"/>
+      <c r="O35" s="58"/>
+      <c r="P35" s="58"/>
+      <c r="Q35" s="58"/>
+      <c r="R35" s="58"/>
+      <c r="S35" s="58"/>
+    </row>
+    <row r="36" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="S24" s="61"/>
-    </row>
-    <row r="25" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="61"/>
-      <c r="L25" s="65"/>
-      <c r="M25" s="65"/>
-      <c r="N25" s="65"/>
-      <c r="O25" s="65"/>
-      <c r="P25" s="65"/>
-      <c r="Q25" s="65"/>
-      <c r="R25" s="61"/>
-      <c r="S25" s="61"/>
-    </row>
-    <row r="26" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="65"/>
-      <c r="M26" s="65"/>
-      <c r="N26" s="65"/>
-      <c r="O26" s="65"/>
-      <c r="P26" s="65"/>
-      <c r="Q26" s="65"/>
-      <c r="R26" s="61"/>
-      <c r="S26" s="61"/>
-    </row>
-    <row r="27" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="65"/>
-      <c r="M27" s="65"/>
-      <c r="N27" s="65"/>
-      <c r="O27" s="65"/>
-      <c r="P27" s="65"/>
-      <c r="Q27" s="65"/>
-      <c r="R27" s="61"/>
-      <c r="S27" s="61"/>
-    </row>
-    <row r="28" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="62" t="s">
+      <c r="C36" s="57"/>
+      <c r="D36" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="62"/>
-      <c r="D28" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="60"/>
-      <c r="P28" s="60"/>
-      <c r="Q28" s="60"/>
-      <c r="R28" s="60"/>
-      <c r="S28" s="60"/>
-    </row>
-    <row r="29" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="60"/>
-      <c r="P29" s="60"/>
-      <c r="Q29" s="60"/>
-      <c r="R29" s="60"/>
-      <c r="S29" s="60"/>
-    </row>
-    <row r="30" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="62"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="60"/>
-      <c r="N30" s="60"/>
-      <c r="O30" s="60"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="60"/>
-      <c r="S30" s="60"/>
-    </row>
-    <row r="31" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="62"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="60"/>
-      <c r="O31" s="60"/>
-      <c r="P31" s="60"/>
-      <c r="Q31" s="60"/>
-      <c r="R31" s="60"/>
-      <c r="S31" s="60"/>
-    </row>
-    <row r="32" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="63" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="63"/>
-      <c r="D32" s="60" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="60"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="60"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="60"/>
-      <c r="L32" s="60"/>
-      <c r="M32" s="60"/>
-      <c r="N32" s="60"/>
-      <c r="O32" s="60"/>
-      <c r="P32" s="60"/>
-      <c r="Q32" s="60"/>
-      <c r="R32" s="60"/>
-      <c r="S32" s="60"/>
-    </row>
-    <row r="33" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="60"/>
-      <c r="P33" s="60"/>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="60"/>
-      <c r="S33" s="60"/>
-    </row>
-    <row r="34" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="60"/>
-      <c r="I34" s="60"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="60"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="60"/>
-      <c r="N34" s="60"/>
-      <c r="O34" s="60"/>
-      <c r="P34" s="60"/>
-      <c r="Q34" s="60"/>
-      <c r="R34" s="60"/>
-      <c r="S34" s="60"/>
-    </row>
-    <row r="35" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="63"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="60"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="60"/>
-      <c r="L35" s="60"/>
-      <c r="M35" s="60"/>
-      <c r="N35" s="60"/>
-      <c r="O35" s="60"/>
-      <c r="P35" s="60"/>
-      <c r="Q35" s="60"/>
-      <c r="R35" s="60"/>
-      <c r="S35" s="60"/>
-    </row>
-    <row r="36" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="59" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="E36" s="60"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="60"/>
-      <c r="I36" s="60"/>
-      <c r="J36" s="60"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="60"/>
-      <c r="N36" s="60"/>
-      <c r="O36" s="60"/>
-      <c r="P36" s="60"/>
-      <c r="Q36" s="60"/>
-      <c r="R36" s="60"/>
-      <c r="S36" s="60"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="58"/>
+      <c r="L36" s="58"/>
+      <c r="M36" s="58"/>
+      <c r="N36" s="58"/>
+      <c r="O36" s="58"/>
+      <c r="P36" s="58"/>
+      <c r="Q36" s="58"/>
+      <c r="R36" s="58"/>
+      <c r="S36" s="58"/>
     </row>
     <row r="37" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="59"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="60"/>
-      <c r="I37" s="60"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="60"/>
-      <c r="L37" s="60"/>
-      <c r="M37" s="60"/>
-      <c r="N37" s="60"/>
-      <c r="O37" s="60"/>
-      <c r="P37" s="60"/>
-      <c r="Q37" s="60"/>
-      <c r="R37" s="60"/>
-      <c r="S37" s="60"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="58"/>
+      <c r="R37" s="58"/>
+      <c r="S37" s="58"/>
     </row>
     <row r="38" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="59"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="60"/>
-      <c r="L38" s="60"/>
-      <c r="M38" s="60"/>
-      <c r="N38" s="60"/>
-      <c r="O38" s="60"/>
-      <c r="P38" s="60"/>
-      <c r="Q38" s="60"/>
-      <c r="R38" s="60"/>
-      <c r="S38" s="60"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="58"/>
+      <c r="I38" s="58"/>
+      <c r="J38" s="58"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
+      <c r="M38" s="58"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="58"/>
+      <c r="P38" s="58"/>
+      <c r="Q38" s="58"/>
+      <c r="R38" s="58"/>
+      <c r="S38" s="58"/>
     </row>
     <row r="39" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="59"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="60"/>
-      <c r="K39" s="60"/>
-      <c r="L39" s="60"/>
-      <c r="M39" s="60"/>
-      <c r="N39" s="60"/>
-      <c r="O39" s="60"/>
-      <c r="P39" s="60"/>
-      <c r="Q39" s="60"/>
-      <c r="R39" s="60"/>
-      <c r="S39" s="60"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="58"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="58"/>
+      <c r="J39" s="58"/>
+      <c r="K39" s="58"/>
+      <c r="L39" s="58"/>
+      <c r="M39" s="58"/>
+      <c r="N39" s="58"/>
+      <c r="O39" s="58"/>
+      <c r="P39" s="58"/>
+      <c r="Q39" s="58"/>
+      <c r="R39" s="58"/>
+      <c r="S39" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="77">
+    <mergeCell ref="B2:R3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
     <mergeCell ref="B36:C39"/>
     <mergeCell ref="D36:S39"/>
     <mergeCell ref="R24:S27"/>
@@ -4140,71 +4182,6 @@
     <mergeCell ref="L24:M27"/>
     <mergeCell ref="N24:O27"/>
     <mergeCell ref="P24:Q27"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="B2:R3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
1.0.200903 100825 Debug Removed PWM channel from memory map and code
</commit_message>
<xml_diff>
--- a/docs/EEPROM map.xlsx
+++ b/docs/EEPROM map.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="110">
   <si>
     <t>Main configuration page</t>
   </si>
@@ -438,12 +438,6 @@
   <si>
     <t>(Protection) Tibia max angle
 (S16) [degree]</t>
-  </si>
-  <si>
-    <t>PWM channel</t>
-  </si>
-  <si>
-    <t>Канал PWM для сервопривода</t>
   </si>
   <si>
     <t>Zero Trim
@@ -983,7 +977,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1087,11 +1081,59 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1102,34 +1144,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1141,9 +1177,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1152,48 +1185,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1578,44 +1569,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
     </row>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -1672,22 +1663,22 @@
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="72"/>
-      <c r="Q6" s="72"/>
-      <c r="R6" s="73"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="42"/>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
@@ -2001,10 +1992,10 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="69" t="s">
+      <c r="Q21" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="R21" s="74"/>
+      <c r="R21" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2032,44 +2023,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
+      <c r="B2" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2257,27 +2248,27 @@
       <c r="C11" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40" t="s">
+      <c r="D11" s="54"/>
+      <c r="E11" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40" t="s">
+      <c r="F11" s="54"/>
+      <c r="G11" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40" t="s">
+      <c r="H11" s="54"/>
+      <c r="I11" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40" t="s">
+      <c r="J11" s="54"/>
+      <c r="K11" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40" t="s">
+      <c r="L11" s="54"/>
+      <c r="M11" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="N11" s="40"/>
+      <c r="N11" s="54"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
@@ -2490,555 +2481,579 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="69" t="s">
+      <c r="Q21" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="R21" s="74"/>
+      <c r="R21" s="45"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43">
+      <c r="C23" s="59"/>
+      <c r="D23" s="59">
         <v>7</v>
       </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43">
+      <c r="E23" s="59"/>
+      <c r="F23" s="59">
         <v>6</v>
       </c>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43">
+      <c r="G23" s="59"/>
+      <c r="H23" s="59">
         <v>5</v>
       </c>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43">
+      <c r="I23" s="59"/>
+      <c r="J23" s="59">
         <v>4</v>
       </c>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43">
+      <c r="K23" s="59"/>
+      <c r="L23" s="59">
         <v>3</v>
       </c>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43">
+      <c r="M23" s="59"/>
+      <c r="N23" s="59">
         <v>2</v>
       </c>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43">
+      <c r="O23" s="59"/>
+      <c r="P23" s="59">
         <v>1</v>
       </c>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43">
+      <c r="Q23" s="59"/>
+      <c r="R23" s="59">
         <v>0</v>
       </c>
-      <c r="S23" s="43"/>
+      <c r="S23" s="59"/>
     </row>
     <row r="24" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42" t="s">
+      <c r="C24" s="57"/>
+      <c r="D24" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
-      <c r="S24" s="42"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="58"/>
+      <c r="Q24" s="58"/>
+      <c r="R24" s="58"/>
+      <c r="S24" s="58"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="42"/>
-      <c r="S25" s="42"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="58"/>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="58"/>
+      <c r="S25" s="58"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="42"/>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
-      <c r="S26" s="42"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="58"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="58"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="58"/>
+      <c r="Q26" s="58"/>
+      <c r="R26" s="58"/>
+      <c r="S26" s="58"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-      <c r="Q27" s="42"/>
-      <c r="R27" s="42"/>
-      <c r="S27" s="42"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="58"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="58"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="58"/>
     </row>
     <row r="28" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45" t="s">
+      <c r="C28" s="55"/>
+      <c r="D28" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="45"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="56"/>
+      <c r="Q30" s="56"/>
+      <c r="R30" s="56"/>
+      <c r="S30" s="56"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="45"/>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
-      <c r="S31" s="45"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="56"/>
+      <c r="S31" s="56"/>
     </row>
     <row r="32" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="42" t="s">
+      <c r="C32" s="57"/>
+      <c r="D32" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="42"/>
-      <c r="M32" s="42"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="42"/>
-      <c r="Q32" s="42"/>
-      <c r="R32" s="42"/>
-      <c r="S32" s="42"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="58"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="58"/>
+      <c r="N32" s="58"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="58"/>
+      <c r="Q32" s="58"/>
+      <c r="R32" s="58"/>
+      <c r="S32" s="58"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="42"/>
-      <c r="L33" s="42"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="42"/>
-      <c r="O33" s="42"/>
-      <c r="P33" s="42"/>
-      <c r="Q33" s="42"/>
-      <c r="R33" s="42"/>
-      <c r="S33" s="42"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="58"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="58"/>
+      <c r="L33" s="58"/>
+      <c r="M33" s="58"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="58"/>
+      <c r="Q33" s="58"/>
+      <c r="R33" s="58"/>
+      <c r="S33" s="58"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="42"/>
-      <c r="Q34" s="42"/>
-      <c r="R34" s="42"/>
-      <c r="S34" s="42"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="58"/>
+      <c r="H34" s="58"/>
+      <c r="I34" s="58"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+      <c r="M34" s="58"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="58"/>
+      <c r="Q34" s="58"/>
+      <c r="R34" s="58"/>
+      <c r="S34" s="58"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42"/>
-      <c r="K35" s="42"/>
-      <c r="L35" s="42"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="42"/>
-      <c r="O35" s="42"/>
-      <c r="P35" s="42"/>
-      <c r="Q35" s="42"/>
-      <c r="R35" s="42"/>
-      <c r="S35" s="42"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="58"/>
+      <c r="J35" s="58"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="58"/>
+      <c r="M35" s="58"/>
+      <c r="N35" s="58"/>
+      <c r="O35" s="58"/>
+      <c r="P35" s="58"/>
+      <c r="Q35" s="58"/>
+      <c r="R35" s="58"/>
+      <c r="S35" s="58"/>
     </row>
     <row r="36" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="45" t="s">
+      <c r="C36" s="55"/>
+      <c r="D36" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="45"/>
-      <c r="R36" s="45"/>
-      <c r="S36" s="45"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="56"/>
+      <c r="K36" s="56"/>
+      <c r="L36" s="56"/>
+      <c r="M36" s="56"/>
+      <c r="N36" s="56"/>
+      <c r="O36" s="56"/>
+      <c r="P36" s="56"/>
+      <c r="Q36" s="56"/>
+      <c r="R36" s="56"/>
+      <c r="S36" s="56"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="45"/>
-      <c r="R37" s="45"/>
-      <c r="S37" s="45"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="56"/>
+      <c r="N37" s="56"/>
+      <c r="O37" s="56"/>
+      <c r="P37" s="56"/>
+      <c r="Q37" s="56"/>
+      <c r="R37" s="56"/>
+      <c r="S37" s="56"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="45"/>
-      <c r="P38" s="45"/>
-      <c r="Q38" s="45"/>
-      <c r="R38" s="45"/>
-      <c r="S38" s="45"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="56"/>
+      <c r="L38" s="56"/>
+      <c r="M38" s="56"/>
+      <c r="N38" s="56"/>
+      <c r="O38" s="56"/>
+      <c r="P38" s="56"/>
+      <c r="Q38" s="56"/>
+      <c r="R38" s="56"/>
+      <c r="S38" s="56"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
-      <c r="P39" s="45"/>
-      <c r="Q39" s="45"/>
-      <c r="R39" s="45"/>
-      <c r="S39" s="45"/>
+      <c r="B39" s="55"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="56"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="56"/>
+      <c r="J39" s="56"/>
+      <c r="K39" s="56"/>
+      <c r="L39" s="56"/>
+      <c r="M39" s="56"/>
+      <c r="N39" s="56"/>
+      <c r="O39" s="56"/>
+      <c r="P39" s="56"/>
+      <c r="Q39" s="56"/>
+      <c r="R39" s="56"/>
+      <c r="S39" s="56"/>
     </row>
     <row r="40" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="41" t="s">
+      <c r="B40" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="42" t="s">
+      <c r="C40" s="57"/>
+      <c r="D40" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="42"/>
-      <c r="J40" s="42"/>
-      <c r="K40" s="42"/>
-      <c r="L40" s="42"/>
-      <c r="M40" s="42"/>
-      <c r="N40" s="42"/>
-      <c r="O40" s="42"/>
-      <c r="P40" s="42"/>
-      <c r="Q40" s="42"/>
-      <c r="R40" s="42"/>
-      <c r="S40" s="42"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="58"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="58"/>
+      <c r="J40" s="58"/>
+      <c r="K40" s="58"/>
+      <c r="L40" s="58"/>
+      <c r="M40" s="58"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="58"/>
+      <c r="Q40" s="58"/>
+      <c r="R40" s="58"/>
+      <c r="S40" s="58"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
-      <c r="K41" s="42"/>
-      <c r="L41" s="42"/>
-      <c r="M41" s="42"/>
-      <c r="N41" s="42"/>
-      <c r="O41" s="42"/>
-      <c r="P41" s="42"/>
-      <c r="Q41" s="42"/>
-      <c r="R41" s="42"/>
-      <c r="S41" s="42"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="58"/>
+      <c r="J41" s="58"/>
+      <c r="K41" s="58"/>
+      <c r="L41" s="58"/>
+      <c r="M41" s="58"/>
+      <c r="N41" s="58"/>
+      <c r="O41" s="58"/>
+      <c r="P41" s="58"/>
+      <c r="Q41" s="58"/>
+      <c r="R41" s="58"/>
+      <c r="S41" s="58"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="42"/>
-      <c r="L42" s="42"/>
-      <c r="M42" s="42"/>
-      <c r="N42" s="42"/>
-      <c r="O42" s="42"/>
-      <c r="P42" s="42"/>
-      <c r="Q42" s="42"/>
-      <c r="R42" s="42"/>
-      <c r="S42" s="42"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="58"/>
+      <c r="L42" s="58"/>
+      <c r="M42" s="58"/>
+      <c r="N42" s="58"/>
+      <c r="O42" s="58"/>
+      <c r="P42" s="58"/>
+      <c r="Q42" s="58"/>
+      <c r="R42" s="58"/>
+      <c r="S42" s="58"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="42"/>
-      <c r="L43" s="42"/>
-      <c r="M43" s="42"/>
-      <c r="N43" s="42"/>
-      <c r="O43" s="42"/>
-      <c r="P43" s="42"/>
-      <c r="Q43" s="42"/>
-      <c r="R43" s="42"/>
-      <c r="S43" s="42"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58"/>
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="58"/>
+      <c r="N43" s="58"/>
+      <c r="O43" s="58"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="58"/>
+      <c r="R43" s="58"/>
+      <c r="S43" s="58"/>
     </row>
     <row r="44" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="44" t="s">
+      <c r="B44" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="45" t="s">
+      <c r="C44" s="55"/>
+      <c r="D44" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="45"/>
-      <c r="M44" s="45"/>
-      <c r="N44" s="45"/>
-      <c r="O44" s="45"/>
-      <c r="P44" s="45"/>
-      <c r="Q44" s="45"/>
-      <c r="R44" s="45"/>
-      <c r="S44" s="45"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="56"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="56"/>
+      <c r="O44" s="56"/>
+      <c r="P44" s="56"/>
+      <c r="Q44" s="56"/>
+      <c r="R44" s="56"/>
+      <c r="S44" s="56"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="45"/>
-      <c r="M45" s="45"/>
-      <c r="N45" s="45"/>
-      <c r="O45" s="45"/>
-      <c r="P45" s="45"/>
-      <c r="Q45" s="45"/>
-      <c r="R45" s="45"/>
-      <c r="S45" s="45"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="56"/>
+      <c r="M45" s="56"/>
+      <c r="N45" s="56"/>
+      <c r="O45" s="56"/>
+      <c r="P45" s="56"/>
+      <c r="Q45" s="56"/>
+      <c r="R45" s="56"/>
+      <c r="S45" s="56"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="45"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="45"/>
-      <c r="M46" s="45"/>
-      <c r="N46" s="45"/>
-      <c r="O46" s="45"/>
-      <c r="P46" s="45"/>
-      <c r="Q46" s="45"/>
-      <c r="R46" s="45"/>
-      <c r="S46" s="45"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="56"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
+      <c r="K46" s="56"/>
+      <c r="L46" s="56"/>
+      <c r="M46" s="56"/>
+      <c r="N46" s="56"/>
+      <c r="O46" s="56"/>
+      <c r="P46" s="56"/>
+      <c r="Q46" s="56"/>
+      <c r="R46" s="56"/>
+      <c r="S46" s="56"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B47" s="44"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
-      <c r="M47" s="45"/>
-      <c r="N47" s="45"/>
-      <c r="O47" s="45"/>
-      <c r="P47" s="45"/>
-      <c r="Q47" s="45"/>
-      <c r="R47" s="45"/>
-      <c r="S47" s="45"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="56"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="56"/>
+      <c r="N47" s="56"/>
+      <c r="O47" s="56"/>
+      <c r="P47" s="56"/>
+      <c r="Q47" s="56"/>
+      <c r="R47" s="56"/>
+      <c r="S47" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="B40:C43"/>
+    <mergeCell ref="D40:S43"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="B24:C27"/>
+    <mergeCell ref="D24:S27"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B44:C47"/>
+    <mergeCell ref="D44:S47"/>
+    <mergeCell ref="B28:C31"/>
+    <mergeCell ref="D28:S31"/>
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="D32:S35"/>
+    <mergeCell ref="B36:C39"/>
+    <mergeCell ref="D36:S39"/>
     <mergeCell ref="Q21:R21"/>
     <mergeCell ref="B2:R3"/>
     <mergeCell ref="C6:D6"/>
@@ -3055,30 +3070,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="B44:C47"/>
-    <mergeCell ref="D44:S47"/>
-    <mergeCell ref="B28:C31"/>
-    <mergeCell ref="D28:S31"/>
-    <mergeCell ref="B32:C35"/>
-    <mergeCell ref="D32:S35"/>
-    <mergeCell ref="B36:C39"/>
-    <mergeCell ref="D36:S39"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="B40:C43"/>
-    <mergeCell ref="D40:S43"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="B24:C27"/>
-    <mergeCell ref="D24:S27"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3090,7 +3081,7 @@
   <sheetPr>
     <tabColor rgb="FFF8A968"/>
   </sheetPr>
-  <dimension ref="B2:V39"/>
+  <dimension ref="B2:V35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3101,44 +3092,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3202,36 +3193,36 @@
       <c r="D6" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="66" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="66"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="61"/>
       <c r="K6" s="34" t="s">
         <v>57</v>
       </c>
       <c r="L6" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="67" t="s">
+      <c r="M6" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="N6" s="67"/>
-      <c r="O6" s="66" t="s">
-        <v>28</v>
-      </c>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="66" t="s">
-        <v>28</v>
-      </c>
-      <c r="R6" s="68"/>
+      <c r="N6" s="62"/>
+      <c r="O6" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="63"/>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
@@ -3243,36 +3234,36 @@
       <c r="D7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="64"/>
-      <c r="G7" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="61"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="64"/>
       <c r="K7" s="32" t="s">
         <v>61</v>
       </c>
       <c r="L7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="63" t="s">
+      <c r="M7" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="N7" s="63"/>
-      <c r="O7" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="R7" s="62"/>
+      <c r="N7" s="66"/>
+      <c r="O7" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="64"/>
+      <c r="Q7" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="65"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
@@ -3284,36 +3275,36 @@
       <c r="D8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="63" t="s">
+      <c r="E8" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="63"/>
-      <c r="G8" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="61"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="64"/>
       <c r="K8" s="33" t="s">
         <v>64</v>
       </c>
       <c r="L8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="64" t="s">
+      <c r="M8" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N8" s="64"/>
-      <c r="O8" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="P8" s="61"/>
-      <c r="Q8" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="R8" s="62"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="64"/>
+      <c r="Q8" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="65"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
@@ -3325,36 +3316,36 @@
       <c r="D9" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="64"/>
-      <c r="G9" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="61"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="64"/>
       <c r="K9" s="32" t="s">
         <v>67</v>
       </c>
       <c r="L9" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="63" t="s">
+      <c r="M9" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="N9" s="63"/>
-      <c r="O9" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="P9" s="61"/>
-      <c r="Q9" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="R9" s="62"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="64"/>
+      <c r="Q9" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="65"/>
     </row>
     <row r="10" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
@@ -3366,36 +3357,36 @@
       <c r="D10" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="63"/>
-      <c r="G10" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="61"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="64"/>
       <c r="K10" s="33" t="s">
         <v>70</v>
       </c>
       <c r="L10" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="64" t="s">
+      <c r="M10" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N10" s="64"/>
-      <c r="O10" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="P10" s="61"/>
-      <c r="Q10" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" s="62"/>
+      <c r="N10" s="67"/>
+      <c r="O10" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="64"/>
+      <c r="Q10" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="65"/>
     </row>
     <row r="11" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
@@ -3407,36 +3398,36 @@
       <c r="D11" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F11" s="64"/>
-      <c r="G11" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="61"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="64"/>
       <c r="K11" s="32" t="s">
         <v>73</v>
       </c>
       <c r="L11" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="63" t="s">
+      <c r="M11" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="N11" s="63"/>
-      <c r="O11" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="R11" s="62"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" s="65"/>
     </row>
     <row r="12" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
@@ -3448,36 +3439,36 @@
       <c r="D12" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="63" t="s">
+      <c r="E12" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="63"/>
-      <c r="G12" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="61"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="64"/>
       <c r="K12" s="33" t="s">
         <v>76</v>
       </c>
       <c r="L12" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M12" s="64" t="s">
+      <c r="M12" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N12" s="64"/>
-      <c r="O12" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="R12" s="62"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" s="65"/>
     </row>
     <row r="13" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
@@ -3489,36 +3480,36 @@
       <c r="D13" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="64" t="s">
+      <c r="E13" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F13" s="64"/>
-      <c r="G13" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="61"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="64"/>
       <c r="K13" s="32" t="s">
         <v>79</v>
       </c>
       <c r="L13" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="63" t="s">
+      <c r="M13" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="N13" s="63"/>
-      <c r="O13" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="R13" s="62"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="64"/>
+      <c r="Q13" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" s="65"/>
     </row>
     <row r="14" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
@@ -3530,36 +3521,36 @@
       <c r="D14" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="63" t="s">
+      <c r="E14" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="F14" s="63"/>
-      <c r="G14" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14" s="61"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="64"/>
       <c r="K14" s="33" t="s">
         <v>93</v>
       </c>
       <c r="L14" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M14" s="64" t="s">
+      <c r="M14" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N14" s="64"/>
-      <c r="O14" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="P14" s="61"/>
-      <c r="Q14" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="R14" s="62"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="64"/>
+      <c r="Q14" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="R14" s="65"/>
     </row>
     <row r="15" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="20" t="s">
@@ -3711,405 +3702,370 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="69" t="s">
+      <c r="Q21" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="R21" s="74"/>
+      <c r="R21" s="45"/>
       <c r="T21" s="21"/>
       <c r="U21" s="21"/>
       <c r="V21" s="21"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43">
+      <c r="C23" s="59"/>
+      <c r="D23" s="59">
         <v>7</v>
       </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43">
+      <c r="E23" s="59"/>
+      <c r="F23" s="59">
         <v>6</v>
       </c>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43">
+      <c r="G23" s="59"/>
+      <c r="H23" s="59">
         <v>5</v>
       </c>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43">
+      <c r="I23" s="59"/>
+      <c r="J23" s="59">
         <v>4</v>
       </c>
-      <c r="K23" s="43"/>
-      <c r="L23" s="43">
+      <c r="K23" s="59"/>
+      <c r="L23" s="59">
         <v>3</v>
       </c>
-      <c r="M23" s="43"/>
-      <c r="N23" s="43">
+      <c r="M23" s="59"/>
+      <c r="N23" s="59">
         <v>2</v>
       </c>
-      <c r="O23" s="43"/>
-      <c r="P23" s="43">
+      <c r="O23" s="59"/>
+      <c r="P23" s="59">
         <v>1</v>
       </c>
-      <c r="Q23" s="43"/>
-      <c r="R23" s="43">
+      <c r="Q23" s="59"/>
+      <c r="R23" s="59">
         <v>0</v>
       </c>
-      <c r="S23" s="43"/>
+      <c r="S23" s="59"/>
     </row>
     <row r="24" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="56" t="s">
+      <c r="C24" s="72"/>
+      <c r="D24" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="M24" s="60"/>
-      <c r="N24" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="O24" s="60"/>
-      <c r="P24" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q24" s="60"/>
-      <c r="R24" s="56" t="s">
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
+      <c r="K24" s="70"/>
+      <c r="L24" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="73"/>
+      <c r="N24" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="73"/>
+      <c r="P24" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" s="73"/>
+      <c r="R24" s="70" t="s">
         <v>89</v>
       </c>
-      <c r="S24" s="56"/>
+      <c r="S24" s="70"/>
     </row>
     <row r="25" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="56"/>
-      <c r="S25" s="56"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="70"/>
+      <c r="K25" s="70"/>
+      <c r="L25" s="73"/>
+      <c r="M25" s="73"/>
+      <c r="N25" s="73"/>
+      <c r="O25" s="73"/>
+      <c r="P25" s="73"/>
+      <c r="Q25" s="73"/>
+      <c r="R25" s="70"/>
+      <c r="S25" s="70"/>
     </row>
     <row r="26" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="56"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="60"/>
-      <c r="N26" s="60"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="56"/>
-      <c r="S26" s="56"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="70"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="73"/>
+      <c r="N26" s="73"/>
+      <c r="O26" s="73"/>
+      <c r="P26" s="73"/>
+      <c r="Q26" s="73"/>
+      <c r="R26" s="70"/>
+      <c r="S26" s="70"/>
     </row>
     <row r="27" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="56"/>
-      <c r="J27" s="56"/>
-      <c r="K27" s="56"/>
-      <c r="L27" s="60"/>
-      <c r="M27" s="60"/>
-      <c r="N27" s="60"/>
-      <c r="O27" s="60"/>
-      <c r="P27" s="60"/>
-      <c r="Q27" s="60"/>
-      <c r="R27" s="56"/>
-      <c r="S27" s="56"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="70"/>
+      <c r="J27" s="70"/>
+      <c r="K27" s="70"/>
+      <c r="L27" s="73"/>
+      <c r="M27" s="73"/>
+      <c r="N27" s="73"/>
+      <c r="O27" s="73"/>
+      <c r="P27" s="73"/>
+      <c r="Q27" s="73"/>
+      <c r="R27" s="70"/>
+      <c r="S27" s="70"/>
     </row>
     <row r="28" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="71" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="55" t="s">
+      <c r="C28" s="71"/>
+      <c r="D28" s="69" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="55"/>
-      <c r="S28" s="55"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="69"/>
+      <c r="M28" s="69"/>
+      <c r="N28" s="69"/>
+      <c r="O28" s="69"/>
+      <c r="P28" s="69"/>
+      <c r="Q28" s="69"/>
+      <c r="R28" s="69"/>
+      <c r="S28" s="69"/>
     </row>
     <row r="29" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="57"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="55"/>
-      <c r="N29" s="55"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="55"/>
-      <c r="R29" s="55"/>
-      <c r="S29" s="55"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="69"/>
+      <c r="M29" s="69"/>
+      <c r="N29" s="69"/>
+      <c r="O29" s="69"/>
+      <c r="P29" s="69"/>
+      <c r="Q29" s="69"/>
+      <c r="R29" s="69"/>
+      <c r="S29" s="69"/>
     </row>
     <row r="30" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="55"/>
-      <c r="M30" s="55"/>
-      <c r="N30" s="55"/>
-      <c r="O30" s="55"/>
-      <c r="P30" s="55"/>
-      <c r="Q30" s="55"/>
-      <c r="R30" s="55"/>
-      <c r="S30" s="55"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="69"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="69"/>
+      <c r="P30" s="69"/>
+      <c r="Q30" s="69"/>
+      <c r="R30" s="69"/>
+      <c r="S30" s="69"/>
     </row>
     <row r="31" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="55"/>
-      <c r="N31" s="55"/>
-      <c r="O31" s="55"/>
-      <c r="P31" s="55"/>
-      <c r="Q31" s="55"/>
-      <c r="R31" s="55"/>
-      <c r="S31" s="55"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
+      <c r="J31" s="69"/>
+      <c r="K31" s="69"/>
+      <c r="L31" s="69"/>
+      <c r="M31" s="69"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="69"/>
+      <c r="Q31" s="69"/>
+      <c r="R31" s="69"/>
+      <c r="S31" s="69"/>
     </row>
     <row r="32" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="58" t="s">
-        <v>109</v>
-      </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="55" t="s">
-        <v>110</v>
-      </c>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="55"/>
-      <c r="M32" s="55"/>
-      <c r="N32" s="55"/>
-      <c r="O32" s="55"/>
-      <c r="P32" s="55"/>
-      <c r="Q32" s="55"/>
-      <c r="R32" s="55"/>
-      <c r="S32" s="55"/>
+      <c r="B32" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="68"/>
+      <c r="D32" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="69"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="69"/>
+      <c r="R32" s="69"/>
+      <c r="S32" s="69"/>
     </row>
     <row r="33" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="58"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="55"/>
-      <c r="E33" s="55"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="55"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="55"/>
-      <c r="M33" s="55"/>
-      <c r="N33" s="55"/>
-      <c r="O33" s="55"/>
-      <c r="P33" s="55"/>
-      <c r="Q33" s="55"/>
-      <c r="R33" s="55"/>
-      <c r="S33" s="55"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="69"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="69"/>
+      <c r="N33" s="69"/>
+      <c r="O33" s="69"/>
+      <c r="P33" s="69"/>
+      <c r="Q33" s="69"/>
+      <c r="R33" s="69"/>
+      <c r="S33" s="69"/>
     </row>
     <row r="34" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55"/>
-      <c r="L34" s="55"/>
-      <c r="M34" s="55"/>
-      <c r="N34" s="55"/>
-      <c r="O34" s="55"/>
-      <c r="P34" s="55"/>
-      <c r="Q34" s="55"/>
-      <c r="R34" s="55"/>
-      <c r="S34" s="55"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
+      <c r="L34" s="69"/>
+      <c r="M34" s="69"/>
+      <c r="N34" s="69"/>
+      <c r="O34" s="69"/>
+      <c r="P34" s="69"/>
+      <c r="Q34" s="69"/>
+      <c r="R34" s="69"/>
+      <c r="S34" s="69"/>
     </row>
     <row r="35" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="55"/>
-      <c r="E35" s="55"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="55"/>
-      <c r="L35" s="55"/>
-      <c r="M35" s="55"/>
-      <c r="N35" s="55"/>
-      <c r="O35" s="55"/>
-      <c r="P35" s="55"/>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="55"/>
-      <c r="S35" s="55"/>
-    </row>
-    <row r="36" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="55"/>
-      <c r="N36" s="55"/>
-      <c r="O36" s="55"/>
-      <c r="P36" s="55"/>
-      <c r="Q36" s="55"/>
-      <c r="R36" s="55"/>
-      <c r="S36" s="55"/>
-    </row>
-    <row r="37" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="54"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="55"/>
-      <c r="M37" s="55"/>
-      <c r="N37" s="55"/>
-      <c r="O37" s="55"/>
-      <c r="P37" s="55"/>
-      <c r="Q37" s="55"/>
-      <c r="R37" s="55"/>
-      <c r="S37" s="55"/>
-    </row>
-    <row r="38" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="55"/>
-      <c r="F38" s="55"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="55"/>
-      <c r="N38" s="55"/>
-      <c r="O38" s="55"/>
-      <c r="P38" s="55"/>
-      <c r="Q38" s="55"/>
-      <c r="R38" s="55"/>
-      <c r="S38" s="55"/>
-    </row>
-    <row r="39" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="54"/>
-      <c r="C39" s="54"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="55"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="55"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
-      <c r="L39" s="55"/>
-      <c r="M39" s="55"/>
-      <c r="N39" s="55"/>
-      <c r="O39" s="55"/>
-      <c r="P39" s="55"/>
-      <c r="Q39" s="55"/>
-      <c r="R39" s="55"/>
-      <c r="S39" s="55"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="69"/>
+      <c r="M35" s="69"/>
+      <c r="N35" s="69"/>
+      <c r="O35" s="69"/>
+      <c r="P35" s="69"/>
+      <c r="Q35" s="69"/>
+      <c r="R35" s="69"/>
+      <c r="S35" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="77">
-    <mergeCell ref="B2:R3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
+  <mergeCells count="75">
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="D32:S35"/>
+    <mergeCell ref="R24:S27"/>
+    <mergeCell ref="B28:C31"/>
+    <mergeCell ref="D28:S31"/>
+    <mergeCell ref="B24:C27"/>
+    <mergeCell ref="D24:K27"/>
+    <mergeCell ref="L24:M27"/>
+    <mergeCell ref="N24:O27"/>
+    <mergeCell ref="P24:Q27"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
     <mergeCell ref="Q7:R7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
@@ -4122,64 +4078,13 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="B36:C39"/>
-    <mergeCell ref="D36:S39"/>
-    <mergeCell ref="R24:S27"/>
-    <mergeCell ref="B28:C31"/>
-    <mergeCell ref="D28:S31"/>
-    <mergeCell ref="B32:C35"/>
-    <mergeCell ref="D32:S35"/>
-    <mergeCell ref="B24:C27"/>
-    <mergeCell ref="D24:K27"/>
-    <mergeCell ref="L24:M27"/>
-    <mergeCell ref="N24:O27"/>
-    <mergeCell ref="P24:Q27"/>
+    <mergeCell ref="B2:R3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added voltage offset to EEPROM Added memory map version check Added print time to logs
</commit_message>
<xml_diff>
--- a/docs/EEPROM map.xlsx
+++ b/docs/EEPROM map.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
   <si>
     <t>Main configuration page</t>
   </si>
@@ -448,6 +448,14 @@
   </si>
   <si>
     <t>Motion core configuration page</t>
+  </si>
+  <si>
+    <t>Memory map version
+(U16)</t>
+  </si>
+  <si>
+    <t>VBAT offset
+(S16) [mV]</t>
   </si>
 </sst>
 </file>
@@ -564,7 +572,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,8 +621,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -973,11 +993,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1081,9 +1127,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1102,6 +1145,24 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1126,48 +1187,6 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1185,6 +1204,42 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1560,7 +1615,9 @@
   </sheetPr>
   <dimension ref="B2:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1569,44 +1626,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
     </row>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -1663,29 +1720,33 @@
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="42"/>
+      <c r="C6" s="73" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="74"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="41"/>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="6"/>
+      <c r="C7" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="76"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1992,15 +2053,17 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="44" t="s">
+      <c r="Q21" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="R21" s="45"/>
+      <c r="R21" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B2:R3"/>
     <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2023,44 +2086,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2118,18 +2181,18 @@
       <c r="B6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47" t="s">
+      <c r="D6" s="52"/>
+      <c r="E6" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47" t="s">
+      <c r="F6" s="52"/>
+      <c r="G6" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="47"/>
+      <c r="H6" s="52"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
       <c r="K6" s="35"/>
@@ -2145,38 +2208,38 @@
       <c r="B7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49" t="s">
+      <c r="D7" s="54"/>
+      <c r="E7" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49" t="s">
+      <c r="F7" s="54"/>
+      <c r="G7" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49" t="s">
+      <c r="H7" s="54"/>
+      <c r="I7" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49" t="s">
+      <c r="J7" s="54"/>
+      <c r="K7" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49" t="s">
+      <c r="L7" s="54"/>
+      <c r="M7" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="N7" s="49"/>
-      <c r="O7" s="50" t="s">
+      <c r="N7" s="54"/>
+      <c r="O7" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="50" t="s">
+      <c r="P7" s="56"/>
+      <c r="Q7" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="R7" s="52"/>
+      <c r="R7" s="57"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
@@ -2245,30 +2308,30 @@
       <c r="B11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54" t="s">
+      <c r="D11" s="45"/>
+      <c r="E11" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54" t="s">
+      <c r="F11" s="45"/>
+      <c r="G11" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54" t="s">
+      <c r="H11" s="45"/>
+      <c r="I11" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54" t="s">
+      <c r="J11" s="45"/>
+      <c r="K11" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="L11" s="54"/>
-      <c r="M11" s="54" t="s">
+      <c r="L11" s="45"/>
+      <c r="M11" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="N11" s="54"/>
+      <c r="N11" s="45"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
@@ -2481,555 +2544,579 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="44" t="s">
+      <c r="Q21" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="R21" s="45"/>
+      <c r="R21" s="44"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59">
+      <c r="C23" s="48"/>
+      <c r="D23" s="48">
         <v>7</v>
       </c>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59">
+      <c r="E23" s="48"/>
+      <c r="F23" s="48">
         <v>6</v>
       </c>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59">
+      <c r="G23" s="48"/>
+      <c r="H23" s="48">
         <v>5</v>
       </c>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59">
+      <c r="I23" s="48"/>
+      <c r="J23" s="48">
         <v>4</v>
       </c>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59">
+      <c r="K23" s="48"/>
+      <c r="L23" s="48">
         <v>3</v>
       </c>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59">
+      <c r="M23" s="48"/>
+      <c r="N23" s="48">
         <v>2</v>
       </c>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59">
+      <c r="O23" s="48"/>
+      <c r="P23" s="48">
         <v>1</v>
       </c>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59">
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48">
         <v>0</v>
       </c>
-      <c r="S23" s="59"/>
+      <c r="S23" s="48"/>
     </row>
     <row r="24" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58" t="s">
+      <c r="C24" s="46"/>
+      <c r="D24" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="58"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="58"/>
-      <c r="O24" s="58"/>
-      <c r="P24" s="58"/>
-      <c r="Q24" s="58"/>
-      <c r="R24" s="58"/>
-      <c r="S24" s="58"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="47"/>
+      <c r="R24" s="47"/>
+      <c r="S24" s="47"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="47"/>
+      <c r="P25" s="47"/>
+      <c r="Q25" s="47"/>
+      <c r="R25" s="47"/>
+      <c r="S25" s="47"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="58"/>
-      <c r="Q26" s="58"/>
-      <c r="R26" s="58"/>
-      <c r="S26" s="58"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="58"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="58"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="47"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="47"/>
     </row>
     <row r="28" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="56" t="s">
+      <c r="C28" s="49"/>
+      <c r="D28" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
-      <c r="K28" s="56"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="56"/>
-      <c r="S28" s="56"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="56"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="56"/>
-      <c r="R29" s="56"/>
-      <c r="S29" s="56"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="50"/>
+      <c r="Q29" s="50"/>
+      <c r="R29" s="50"/>
+      <c r="S29" s="50"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
-      <c r="K30" s="56"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="56"/>
-      <c r="N30" s="56"/>
-      <c r="O30" s="56"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="56"/>
-      <c r="S30" s="56"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="50"/>
+      <c r="P31" s="50"/>
+      <c r="Q31" s="50"/>
+      <c r="R31" s="50"/>
+      <c r="S31" s="50"/>
     </row>
     <row r="32" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="57" t="s">
+      <c r="B32" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58" t="s">
+      <c r="C32" s="46"/>
+      <c r="D32" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="58"/>
-      <c r="Q32" s="58"/>
-      <c r="R32" s="58"/>
-      <c r="S32" s="58"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="47"/>
+      <c r="P32" s="47"/>
+      <c r="Q32" s="47"/>
+      <c r="R32" s="47"/>
+      <c r="S32" s="47"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="58"/>
-      <c r="R33" s="58"/>
-      <c r="S33" s="58"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="47"/>
+      <c r="O33" s="47"/>
+      <c r="P33" s="47"/>
+      <c r="Q33" s="47"/>
+      <c r="R33" s="47"/>
+      <c r="S33" s="47"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="58"/>
-      <c r="S34" s="58"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
+      <c r="P34" s="47"/>
+      <c r="Q34" s="47"/>
+      <c r="R34" s="47"/>
+      <c r="S34" s="47"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
-      <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
-      <c r="R35" s="58"/>
-      <c r="S35" s="58"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
+      <c r="Q35" s="47"/>
+      <c r="R35" s="47"/>
+      <c r="S35" s="47"/>
     </row>
     <row r="36" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="55" t="s">
+      <c r="B36" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="55"/>
-      <c r="D36" s="56" t="s">
+      <c r="C36" s="49"/>
+      <c r="D36" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="56"/>
-      <c r="K36" s="56"/>
-      <c r="L36" s="56"/>
-      <c r="M36" s="56"/>
-      <c r="N36" s="56"/>
-      <c r="O36" s="56"/>
-      <c r="P36" s="56"/>
-      <c r="Q36" s="56"/>
-      <c r="R36" s="56"/>
-      <c r="S36" s="56"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="50"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="50"/>
+      <c r="Q36" s="50"/>
+      <c r="R36" s="50"/>
+      <c r="S36" s="50"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
-      <c r="R37" s="56"/>
-      <c r="S37" s="56"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="50"/>
+      <c r="P37" s="50"/>
+      <c r="Q37" s="50"/>
+      <c r="R37" s="50"/>
+      <c r="S37" s="50"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="56"/>
-      <c r="K38" s="56"/>
-      <c r="L38" s="56"/>
-      <c r="M38" s="56"/>
-      <c r="N38" s="56"/>
-      <c r="O38" s="56"/>
-      <c r="P38" s="56"/>
-      <c r="Q38" s="56"/>
-      <c r="R38" s="56"/>
-      <c r="S38" s="56"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="50"/>
+      <c r="P38" s="50"/>
+      <c r="Q38" s="50"/>
+      <c r="R38" s="50"/>
+      <c r="S38" s="50"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="56"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="56"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="56"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="56"/>
-      <c r="R39" s="56"/>
-      <c r="S39" s="56"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="50"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="50"/>
+      <c r="P39" s="50"/>
+      <c r="Q39" s="50"/>
+      <c r="R39" s="50"/>
+      <c r="S39" s="50"/>
     </row>
     <row r="40" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="57" t="s">
+      <c r="B40" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="D40" s="58" t="s">
+      <c r="C40" s="46"/>
+      <c r="D40" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E40" s="58"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="58"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="58"/>
-      <c r="K40" s="58"/>
-      <c r="L40" s="58"/>
-      <c r="M40" s="58"/>
-      <c r="N40" s="58"/>
-      <c r="O40" s="58"/>
-      <c r="P40" s="58"/>
-      <c r="Q40" s="58"/>
-      <c r="R40" s="58"/>
-      <c r="S40" s="58"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="47"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="47"/>
+      <c r="M40" s="47"/>
+      <c r="N40" s="47"/>
+      <c r="O40" s="47"/>
+      <c r="P40" s="47"/>
+      <c r="Q40" s="47"/>
+      <c r="R40" s="47"/>
+      <c r="S40" s="47"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B41" s="57"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="58"/>
-      <c r="K41" s="58"/>
-      <c r="L41" s="58"/>
-      <c r="M41" s="58"/>
-      <c r="N41" s="58"/>
-      <c r="O41" s="58"/>
-      <c r="P41" s="58"/>
-      <c r="Q41" s="58"/>
-      <c r="R41" s="58"/>
-      <c r="S41" s="58"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="47"/>
+      <c r="L41" s="47"/>
+      <c r="M41" s="47"/>
+      <c r="N41" s="47"/>
+      <c r="O41" s="47"/>
+      <c r="P41" s="47"/>
+      <c r="Q41" s="47"/>
+      <c r="R41" s="47"/>
+      <c r="S41" s="47"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="57"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="58"/>
-      <c r="K42" s="58"/>
-      <c r="L42" s="58"/>
-      <c r="M42" s="58"/>
-      <c r="N42" s="58"/>
-      <c r="O42" s="58"/>
-      <c r="P42" s="58"/>
-      <c r="Q42" s="58"/>
-      <c r="R42" s="58"/>
-      <c r="S42" s="58"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="47"/>
+      <c r="N42" s="47"/>
+      <c r="O42" s="47"/>
+      <c r="P42" s="47"/>
+      <c r="Q42" s="47"/>
+      <c r="R42" s="47"/>
+      <c r="S42" s="47"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B43" s="57"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="58"/>
-      <c r="L43" s="58"/>
-      <c r="M43" s="58"/>
-      <c r="N43" s="58"/>
-      <c r="O43" s="58"/>
-      <c r="P43" s="58"/>
-      <c r="Q43" s="58"/>
-      <c r="R43" s="58"/>
-      <c r="S43" s="58"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="47"/>
+      <c r="N43" s="47"/>
+      <c r="O43" s="47"/>
+      <c r="P43" s="47"/>
+      <c r="Q43" s="47"/>
+      <c r="R43" s="47"/>
+      <c r="S43" s="47"/>
     </row>
     <row r="44" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="55" t="s">
+      <c r="B44" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C44" s="55"/>
-      <c r="D44" s="56" t="s">
+      <c r="C44" s="49"/>
+      <c r="D44" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="56"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="56"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="56"/>
-      <c r="O44" s="56"/>
-      <c r="P44" s="56"/>
-      <c r="Q44" s="56"/>
-      <c r="R44" s="56"/>
-      <c r="S44" s="56"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
+      <c r="R44" s="50"/>
+      <c r="S44" s="50"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="56"/>
-      <c r="O45" s="56"/>
-      <c r="P45" s="56"/>
-      <c r="Q45" s="56"/>
-      <c r="R45" s="56"/>
-      <c r="S45" s="56"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="50"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="50"/>
+      <c r="P45" s="50"/>
+      <c r="Q45" s="50"/>
+      <c r="R45" s="50"/>
+      <c r="S45" s="50"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="56"/>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="56"/>
-      <c r="O46" s="56"/>
-      <c r="P46" s="56"/>
-      <c r="Q46" s="56"/>
-      <c r="R46" s="56"/>
-      <c r="S46" s="56"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="50"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="50"/>
+      <c r="P46" s="50"/>
+      <c r="Q46" s="50"/>
+      <c r="R46" s="50"/>
+      <c r="S46" s="50"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B47" s="55"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="56"/>
-      <c r="L47" s="56"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="56"/>
-      <c r="O47" s="56"/>
-      <c r="P47" s="56"/>
-      <c r="Q47" s="56"/>
-      <c r="R47" s="56"/>
-      <c r="S47" s="56"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="50"/>
+      <c r="M47" s="50"/>
+      <c r="N47" s="50"/>
+      <c r="O47" s="50"/>
+      <c r="P47" s="50"/>
+      <c r="Q47" s="50"/>
+      <c r="R47" s="50"/>
+      <c r="S47" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="B2:R3"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B44:C47"/>
+    <mergeCell ref="D44:S47"/>
+    <mergeCell ref="B28:C31"/>
+    <mergeCell ref="D28:S31"/>
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="D32:S35"/>
+    <mergeCell ref="B36:C39"/>
+    <mergeCell ref="D36:S39"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="M11:N11"/>
@@ -3046,30 +3133,6 @@
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="J23:K23"/>
-    <mergeCell ref="B44:C47"/>
-    <mergeCell ref="D44:S47"/>
-    <mergeCell ref="B28:C31"/>
-    <mergeCell ref="D28:S31"/>
-    <mergeCell ref="B32:C35"/>
-    <mergeCell ref="D32:S35"/>
-    <mergeCell ref="B36:C39"/>
-    <mergeCell ref="D36:S39"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="B2:R3"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3092,44 +3155,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3193,36 +3256,36 @@
       <c r="D6" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="61"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="70"/>
       <c r="K6" s="34" t="s">
         <v>57</v>
       </c>
       <c r="L6" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="62" t="s">
+      <c r="M6" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="N6" s="62"/>
-      <c r="O6" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="P6" s="61"/>
-      <c r="Q6" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="R6" s="63"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="72"/>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
@@ -3234,36 +3297,36 @@
       <c r="D7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="67"/>
-      <c r="G7" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="64"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="65"/>
       <c r="K7" s="32" t="s">
         <v>61</v>
       </c>
       <c r="L7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="66" t="s">
+      <c r="M7" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N7" s="66"/>
-      <c r="O7" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R7" s="65"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="66"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
@@ -3275,36 +3338,36 @@
       <c r="D8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="66"/>
-      <c r="G8" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="64"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="65"/>
       <c r="K8" s="33" t="s">
         <v>64</v>
       </c>
       <c r="L8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="67" t="s">
+      <c r="M8" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="N8" s="67"/>
-      <c r="O8" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R8" s="65"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="66"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
@@ -3316,36 +3379,36 @@
       <c r="D9" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="64"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="65"/>
       <c r="K9" s="32" t="s">
         <v>67</v>
       </c>
       <c r="L9" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="66" t="s">
+      <c r="M9" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N9" s="66"/>
-      <c r="O9" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R9" s="65"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="66"/>
     </row>
     <row r="10" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
@@ -3357,36 +3420,36 @@
       <c r="D10" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="66"/>
-      <c r="G10" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="64"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="65"/>
       <c r="K10" s="33" t="s">
         <v>70</v>
       </c>
       <c r="L10" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="67" t="s">
+      <c r="M10" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="N10" s="67"/>
-      <c r="O10" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" s="65"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="66"/>
     </row>
     <row r="11" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
@@ -3398,36 +3461,36 @@
       <c r="D11" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="67" t="s">
+      <c r="E11" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="F11" s="67"/>
-      <c r="G11" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="64"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="65"/>
       <c r="K11" s="32" t="s">
         <v>73</v>
       </c>
       <c r="L11" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="66" t="s">
+      <c r="M11" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N11" s="66"/>
-      <c r="O11" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P11" s="64"/>
-      <c r="Q11" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R11" s="65"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" s="66"/>
     </row>
     <row r="12" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
@@ -3439,36 +3502,36 @@
       <c r="D12" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="66" t="s">
+      <c r="E12" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="66"/>
-      <c r="G12" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="64"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="65"/>
       <c r="K12" s="33" t="s">
         <v>76</v>
       </c>
       <c r="L12" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M12" s="67" t="s">
+      <c r="M12" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="N12" s="67"/>
-      <c r="O12" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R12" s="65"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" s="66"/>
     </row>
     <row r="13" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
@@ -3480,36 +3543,36 @@
       <c r="D13" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="67" t="s">
+      <c r="E13" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="F13" s="67"/>
-      <c r="G13" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="64"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="65"/>
       <c r="K13" s="32" t="s">
         <v>79</v>
       </c>
       <c r="L13" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="66" t="s">
+      <c r="M13" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N13" s="66"/>
-      <c r="O13" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R13" s="65"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" s="66"/>
     </row>
     <row r="14" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
@@ -3521,36 +3584,36 @@
       <c r="D14" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F14" s="66"/>
-      <c r="G14" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14" s="64"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="65"/>
       <c r="K14" s="33" t="s">
         <v>93</v>
       </c>
       <c r="L14" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M14" s="67" t="s">
+      <c r="M14" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="N14" s="67"/>
-      <c r="O14" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R14" s="65"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R14" s="66"/>
     </row>
     <row r="15" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="20" t="s">
@@ -3702,334 +3765,357 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="44" t="s">
+      <c r="Q21" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="R21" s="45"/>
+      <c r="R21" s="44"/>
       <c r="T21" s="21"/>
       <c r="U21" s="21"/>
       <c r="V21" s="21"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59">
+      <c r="C23" s="48"/>
+      <c r="D23" s="48">
         <v>7</v>
       </c>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59">
+      <c r="E23" s="48"/>
+      <c r="F23" s="48">
         <v>6</v>
       </c>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59">
+      <c r="G23" s="48"/>
+      <c r="H23" s="48">
         <v>5</v>
       </c>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59">
+      <c r="I23" s="48"/>
+      <c r="J23" s="48">
         <v>4</v>
       </c>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59">
+      <c r="K23" s="48"/>
+      <c r="L23" s="48">
         <v>3</v>
       </c>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59">
+      <c r="M23" s="48"/>
+      <c r="N23" s="48">
         <v>2</v>
       </c>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59">
+      <c r="O23" s="48"/>
+      <c r="P23" s="48">
         <v>1</v>
       </c>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59">
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48">
         <v>0</v>
       </c>
-      <c r="S23" s="59"/>
+      <c r="S23" s="48"/>
     </row>
     <row r="24" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="70" t="s">
+      <c r="C24" s="63"/>
+      <c r="D24" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="70"/>
-      <c r="J24" s="70"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="73" t="s">
-        <v>28</v>
-      </c>
-      <c r="M24" s="73"/>
-      <c r="N24" s="73" t="s">
-        <v>28</v>
-      </c>
-      <c r="O24" s="73"/>
-      <c r="P24" s="73" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q24" s="73"/>
-      <c r="R24" s="70" t="s">
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="64"/>
+      <c r="P24" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="S24" s="70"/>
+      <c r="S24" s="61"/>
     </row>
     <row r="25" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="70"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="70"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="73"/>
-      <c r="N25" s="73"/>
-      <c r="O25" s="73"/>
-      <c r="P25" s="73"/>
-      <c r="Q25" s="73"/>
-      <c r="R25" s="70"/>
-      <c r="S25" s="70"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="64"/>
+      <c r="Q25" s="64"/>
+      <c r="R25" s="61"/>
+      <c r="S25" s="61"/>
     </row>
     <row r="26" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="73"/>
-      <c r="M26" s="73"/>
-      <c r="N26" s="73"/>
-      <c r="O26" s="73"/>
-      <c r="P26" s="73"/>
-      <c r="Q26" s="73"/>
-      <c r="R26" s="70"/>
-      <c r="S26" s="70"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="64"/>
+      <c r="P26" s="64"/>
+      <c r="Q26" s="64"/>
+      <c r="R26" s="61"/>
+      <c r="S26" s="61"/>
     </row>
     <row r="27" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="70"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="73"/>
-      <c r="M27" s="73"/>
-      <c r="N27" s="73"/>
-      <c r="O27" s="73"/>
-      <c r="P27" s="73"/>
-      <c r="Q27" s="73"/>
-      <c r="R27" s="70"/>
-      <c r="S27" s="70"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="64"/>
+      <c r="P27" s="64"/>
+      <c r="Q27" s="64"/>
+      <c r="R27" s="61"/>
+      <c r="S27" s="61"/>
     </row>
     <row r="28" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="71" t="s">
+      <c r="B28" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="71"/>
-      <c r="D28" s="69" t="s">
+      <c r="C28" s="62"/>
+      <c r="D28" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="69"/>
-      <c r="N28" s="69"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="69"/>
-      <c r="Q28" s="69"/>
-      <c r="R28" s="69"/>
-      <c r="S28" s="69"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="60"/>
+      <c r="R28" s="60"/>
+      <c r="S28" s="60"/>
     </row>
     <row r="29" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="69"/>
-      <c r="M29" s="69"/>
-      <c r="N29" s="69"/>
-      <c r="O29" s="69"/>
-      <c r="P29" s="69"/>
-      <c r="Q29" s="69"/>
-      <c r="R29" s="69"/>
-      <c r="S29" s="69"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
+      <c r="P29" s="60"/>
+      <c r="Q29" s="60"/>
+      <c r="R29" s="60"/>
+      <c r="S29" s="60"/>
     </row>
     <row r="30" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="69"/>
-      <c r="N30" s="69"/>
-      <c r="O30" s="69"/>
-      <c r="P30" s="69"/>
-      <c r="Q30" s="69"/>
-      <c r="R30" s="69"/>
-      <c r="S30" s="69"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="60"/>
+      <c r="S30" s="60"/>
     </row>
     <row r="31" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="71"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="69"/>
-      <c r="N31" s="69"/>
-      <c r="O31" s="69"/>
-      <c r="P31" s="69"/>
-      <c r="Q31" s="69"/>
-      <c r="R31" s="69"/>
-      <c r="S31" s="69"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="60"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="60"/>
+      <c r="P31" s="60"/>
+      <c r="Q31" s="60"/>
+      <c r="R31" s="60"/>
+      <c r="S31" s="60"/>
     </row>
     <row r="32" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="68"/>
-      <c r="D32" s="69" t="s">
+      <c r="C32" s="59"/>
+      <c r="D32" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
-      <c r="N32" s="69"/>
-      <c r="O32" s="69"/>
-      <c r="P32" s="69"/>
-      <c r="Q32" s="69"/>
-      <c r="R32" s="69"/>
-      <c r="S32" s="69"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="60"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="60"/>
+      <c r="R32" s="60"/>
+      <c r="S32" s="60"/>
     </row>
     <row r="33" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="69"/>
-      <c r="N33" s="69"/>
-      <c r="O33" s="69"/>
-      <c r="P33" s="69"/>
-      <c r="Q33" s="69"/>
-      <c r="R33" s="69"/>
-      <c r="S33" s="69"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="60"/>
     </row>
     <row r="34" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
-      <c r="L34" s="69"/>
-      <c r="M34" s="69"/>
-      <c r="N34" s="69"/>
-      <c r="O34" s="69"/>
-      <c r="P34" s="69"/>
-      <c r="Q34" s="69"/>
-      <c r="R34" s="69"/>
-      <c r="S34" s="69"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="60"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="60"/>
+      <c r="S34" s="60"/>
     </row>
     <row r="35" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="68"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="69"/>
-      <c r="L35" s="69"/>
-      <c r="M35" s="69"/>
-      <c r="N35" s="69"/>
-      <c r="O35" s="69"/>
-      <c r="P35" s="69"/>
-      <c r="Q35" s="69"/>
-      <c r="R35" s="69"/>
-      <c r="S35" s="69"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="60"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B32:C35"/>
-    <mergeCell ref="D32:S35"/>
-    <mergeCell ref="R24:S27"/>
-    <mergeCell ref="B28:C31"/>
-    <mergeCell ref="D28:S31"/>
-    <mergeCell ref="B24:C27"/>
-    <mergeCell ref="D24:K27"/>
-    <mergeCell ref="L24:M27"/>
-    <mergeCell ref="N24:O27"/>
-    <mergeCell ref="P24:Q27"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B2:R3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
     <mergeCell ref="Q13:R13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
@@ -4042,49 +4128,26 @@
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="B2:R3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="D32:S35"/>
+    <mergeCell ref="R24:S27"/>
+    <mergeCell ref="B28:C31"/>
+    <mergeCell ref="D28:S31"/>
+    <mergeCell ref="B24:C27"/>
+    <mergeCell ref="D24:K27"/>
+    <mergeCell ref="L24:M27"/>
+    <mergeCell ref="N24:O27"/>
+    <mergeCell ref="P24:Q27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes for v1.01 (#43)
- Split limp 3 to two pars
- Added place for load cell
- Added place for HX711
- Added sensor MCU
- Added connectors for HX711
- Moved LEDs connector
- Connect SMCU to MCU
- Added stabilization by axis X and Z
- Updated math: removed time step
</commit_message>
<xml_diff>
--- a/docs/EEPROM map.xlsx
+++ b/docs/EEPROM map.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
   <si>
     <t>Main configuration page</t>
   </si>
@@ -448,6 +448,14 @@
   </si>
   <si>
     <t>Motion core configuration page</t>
+  </si>
+  <si>
+    <t>Memory map version
+(U16)</t>
+  </si>
+  <si>
+    <t>VBAT offset
+(S16) [mV]</t>
   </si>
 </sst>
 </file>
@@ -564,7 +572,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -613,8 +621,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -973,11 +993,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1081,9 +1127,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1102,6 +1145,24 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1126,48 +1187,6 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1185,6 +1204,42 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1560,7 +1615,9 @@
   </sheetPr>
   <dimension ref="B2:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1569,44 +1626,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
     </row>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -1663,29 +1720,33 @@
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40"/>
-      <c r="O6" s="40"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="42"/>
+      <c r="C6" s="73" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="74"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="41"/>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="6"/>
+      <c r="C7" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="76"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1992,15 +2053,17 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="44" t="s">
+      <c r="Q21" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="R21" s="45"/>
+      <c r="R21" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B2:R3"/>
     <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2023,44 +2086,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2118,18 +2181,18 @@
       <c r="B6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47" t="s">
+      <c r="D6" s="52"/>
+      <c r="E6" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47" t="s">
+      <c r="F6" s="52"/>
+      <c r="G6" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="47"/>
+      <c r="H6" s="52"/>
       <c r="I6" s="35"/>
       <c r="J6" s="35"/>
       <c r="K6" s="35"/>
@@ -2145,38 +2208,38 @@
       <c r="B7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49" t="s">
+      <c r="D7" s="54"/>
+      <c r="E7" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49" t="s">
+      <c r="F7" s="54"/>
+      <c r="G7" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49" t="s">
+      <c r="H7" s="54"/>
+      <c r="I7" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49" t="s">
+      <c r="J7" s="54"/>
+      <c r="K7" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49" t="s">
+      <c r="L7" s="54"/>
+      <c r="M7" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="N7" s="49"/>
-      <c r="O7" s="50" t="s">
+      <c r="N7" s="54"/>
+      <c r="O7" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="50" t="s">
+      <c r="P7" s="56"/>
+      <c r="Q7" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="R7" s="52"/>
+      <c r="R7" s="57"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
@@ -2245,30 +2308,30 @@
       <c r="B11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54" t="s">
+      <c r="D11" s="45"/>
+      <c r="E11" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54" t="s">
+      <c r="F11" s="45"/>
+      <c r="G11" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54" t="s">
+      <c r="H11" s="45"/>
+      <c r="I11" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54" t="s">
+      <c r="J11" s="45"/>
+      <c r="K11" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="L11" s="54"/>
-      <c r="M11" s="54" t="s">
+      <c r="L11" s="45"/>
+      <c r="M11" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="N11" s="54"/>
+      <c r="N11" s="45"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
@@ -2481,555 +2544,579 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="44" t="s">
+      <c r="Q21" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="R21" s="45"/>
+      <c r="R21" s="44"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59">
+      <c r="C23" s="48"/>
+      <c r="D23" s="48">
         <v>7</v>
       </c>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59">
+      <c r="E23" s="48"/>
+      <c r="F23" s="48">
         <v>6</v>
       </c>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59">
+      <c r="G23" s="48"/>
+      <c r="H23" s="48">
         <v>5</v>
       </c>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59">
+      <c r="I23" s="48"/>
+      <c r="J23" s="48">
         <v>4</v>
       </c>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59">
+      <c r="K23" s="48"/>
+      <c r="L23" s="48">
         <v>3</v>
       </c>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59">
+      <c r="M23" s="48"/>
+      <c r="N23" s="48">
         <v>2</v>
       </c>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59">
+      <c r="O23" s="48"/>
+      <c r="P23" s="48">
         <v>1</v>
       </c>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59">
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48">
         <v>0</v>
       </c>
-      <c r="S23" s="59"/>
+      <c r="S23" s="48"/>
     </row>
     <row r="24" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58" t="s">
+      <c r="C24" s="46"/>
+      <c r="D24" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="58"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="58"/>
-      <c r="O24" s="58"/>
-      <c r="P24" s="58"/>
-      <c r="Q24" s="58"/>
-      <c r="R24" s="58"/>
-      <c r="S24" s="58"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="47"/>
+      <c r="R24" s="47"/>
+      <c r="S24" s="47"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="58"/>
-      <c r="L25" s="58"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="58"/>
-      <c r="S25" s="58"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="47"/>
+      <c r="P25" s="47"/>
+      <c r="Q25" s="47"/>
+      <c r="R25" s="47"/>
+      <c r="S25" s="47"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="58"/>
-      <c r="Q26" s="58"/>
-      <c r="R26" s="58"/>
-      <c r="S26" s="58"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="58"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="58"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="47"/>
+      <c r="K27" s="47"/>
+      <c r="L27" s="47"/>
+      <c r="M27" s="47"/>
+      <c r="N27" s="47"/>
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="47"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="47"/>
     </row>
     <row r="28" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="56" t="s">
+      <c r="C28" s="49"/>
+      <c r="D28" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
-      <c r="K28" s="56"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
-      <c r="R28" s="56"/>
-      <c r="S28" s="56"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="56"/>
-      <c r="K29" s="56"/>
-      <c r="L29" s="56"/>
-      <c r="M29" s="56"/>
-      <c r="N29" s="56"/>
-      <c r="O29" s="56"/>
-      <c r="P29" s="56"/>
-      <c r="Q29" s="56"/>
-      <c r="R29" s="56"/>
-      <c r="S29" s="56"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="50"/>
+      <c r="Q29" s="50"/>
+      <c r="R29" s="50"/>
+      <c r="S29" s="50"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
-      <c r="K30" s="56"/>
-      <c r="L30" s="56"/>
-      <c r="M30" s="56"/>
-      <c r="N30" s="56"/>
-      <c r="O30" s="56"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="56"/>
-      <c r="S30" s="56"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="50"/>
+      <c r="P31" s="50"/>
+      <c r="Q31" s="50"/>
+      <c r="R31" s="50"/>
+      <c r="S31" s="50"/>
     </row>
     <row r="32" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="57" t="s">
+      <c r="B32" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58" t="s">
+      <c r="C32" s="46"/>
+      <c r="D32" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="58"/>
-      <c r="Q32" s="58"/>
-      <c r="R32" s="58"/>
-      <c r="S32" s="58"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="47"/>
+      <c r="P32" s="47"/>
+      <c r="Q32" s="47"/>
+      <c r="R32" s="47"/>
+      <c r="S32" s="47"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="58"/>
-      <c r="R33" s="58"/>
-      <c r="S33" s="58"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="47"/>
+      <c r="O33" s="47"/>
+      <c r="P33" s="47"/>
+      <c r="Q33" s="47"/>
+      <c r="R33" s="47"/>
+      <c r="S33" s="47"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="58"/>
-      <c r="S34" s="58"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
+      <c r="P34" s="47"/>
+      <c r="Q34" s="47"/>
+      <c r="R34" s="47"/>
+      <c r="S34" s="47"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
-      <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
-      <c r="R35" s="58"/>
-      <c r="S35" s="58"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
+      <c r="Q35" s="47"/>
+      <c r="R35" s="47"/>
+      <c r="S35" s="47"/>
     </row>
     <row r="36" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="55" t="s">
+      <c r="B36" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="55"/>
-      <c r="D36" s="56" t="s">
+      <c r="C36" s="49"/>
+      <c r="D36" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="56"/>
-      <c r="K36" s="56"/>
-      <c r="L36" s="56"/>
-      <c r="M36" s="56"/>
-      <c r="N36" s="56"/>
-      <c r="O36" s="56"/>
-      <c r="P36" s="56"/>
-      <c r="Q36" s="56"/>
-      <c r="R36" s="56"/>
-      <c r="S36" s="56"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="50"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="50"/>
+      <c r="Q36" s="50"/>
+      <c r="R36" s="50"/>
+      <c r="S36" s="50"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="56"/>
-      <c r="O37" s="56"/>
-      <c r="P37" s="56"/>
-      <c r="Q37" s="56"/>
-      <c r="R37" s="56"/>
-      <c r="S37" s="56"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="50"/>
+      <c r="P37" s="50"/>
+      <c r="Q37" s="50"/>
+      <c r="R37" s="50"/>
+      <c r="S37" s="50"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="56"/>
-      <c r="K38" s="56"/>
-      <c r="L38" s="56"/>
-      <c r="M38" s="56"/>
-      <c r="N38" s="56"/>
-      <c r="O38" s="56"/>
-      <c r="P38" s="56"/>
-      <c r="Q38" s="56"/>
-      <c r="R38" s="56"/>
-      <c r="S38" s="56"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="50"/>
+      <c r="P38" s="50"/>
+      <c r="Q38" s="50"/>
+      <c r="R38" s="50"/>
+      <c r="S38" s="50"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="56"/>
-      <c r="J39" s="56"/>
-      <c r="K39" s="56"/>
-      <c r="L39" s="56"/>
-      <c r="M39" s="56"/>
-      <c r="N39" s="56"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="56"/>
-      <c r="Q39" s="56"/>
-      <c r="R39" s="56"/>
-      <c r="S39" s="56"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="50"/>
+      <c r="K39" s="50"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="50"/>
+      <c r="P39" s="50"/>
+      <c r="Q39" s="50"/>
+      <c r="R39" s="50"/>
+      <c r="S39" s="50"/>
     </row>
     <row r="40" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="57" t="s">
+      <c r="B40" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="57"/>
-      <c r="D40" s="58" t="s">
+      <c r="C40" s="46"/>
+      <c r="D40" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E40" s="58"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="58"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="58"/>
-      <c r="K40" s="58"/>
-      <c r="L40" s="58"/>
-      <c r="M40" s="58"/>
-      <c r="N40" s="58"/>
-      <c r="O40" s="58"/>
-      <c r="P40" s="58"/>
-      <c r="Q40" s="58"/>
-      <c r="R40" s="58"/>
-      <c r="S40" s="58"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="47"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="47"/>
+      <c r="M40" s="47"/>
+      <c r="N40" s="47"/>
+      <c r="O40" s="47"/>
+      <c r="P40" s="47"/>
+      <c r="Q40" s="47"/>
+      <c r="R40" s="47"/>
+      <c r="S40" s="47"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B41" s="57"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="58"/>
-      <c r="K41" s="58"/>
-      <c r="L41" s="58"/>
-      <c r="M41" s="58"/>
-      <c r="N41" s="58"/>
-      <c r="O41" s="58"/>
-      <c r="P41" s="58"/>
-      <c r="Q41" s="58"/>
-      <c r="R41" s="58"/>
-      <c r="S41" s="58"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="47"/>
+      <c r="L41" s="47"/>
+      <c r="M41" s="47"/>
+      <c r="N41" s="47"/>
+      <c r="O41" s="47"/>
+      <c r="P41" s="47"/>
+      <c r="Q41" s="47"/>
+      <c r="R41" s="47"/>
+      <c r="S41" s="47"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="57"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="58"/>
-      <c r="K42" s="58"/>
-      <c r="L42" s="58"/>
-      <c r="M42" s="58"/>
-      <c r="N42" s="58"/>
-      <c r="O42" s="58"/>
-      <c r="P42" s="58"/>
-      <c r="Q42" s="58"/>
-      <c r="R42" s="58"/>
-      <c r="S42" s="58"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="47"/>
+      <c r="N42" s="47"/>
+      <c r="O42" s="47"/>
+      <c r="P42" s="47"/>
+      <c r="Q42" s="47"/>
+      <c r="R42" s="47"/>
+      <c r="S42" s="47"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B43" s="57"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="58"/>
-      <c r="L43" s="58"/>
-      <c r="M43" s="58"/>
-      <c r="N43" s="58"/>
-      <c r="O43" s="58"/>
-      <c r="P43" s="58"/>
-      <c r="Q43" s="58"/>
-      <c r="R43" s="58"/>
-      <c r="S43" s="58"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="47"/>
+      <c r="N43" s="47"/>
+      <c r="O43" s="47"/>
+      <c r="P43" s="47"/>
+      <c r="Q43" s="47"/>
+      <c r="R43" s="47"/>
+      <c r="S43" s="47"/>
     </row>
     <row r="44" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="55" t="s">
+      <c r="B44" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C44" s="55"/>
-      <c r="D44" s="56" t="s">
+      <c r="C44" s="49"/>
+      <c r="D44" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="56"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="56"/>
-      <c r="L44" s="56"/>
-      <c r="M44" s="56"/>
-      <c r="N44" s="56"/>
-      <c r="O44" s="56"/>
-      <c r="P44" s="56"/>
-      <c r="Q44" s="56"/>
-      <c r="R44" s="56"/>
-      <c r="S44" s="56"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
+      <c r="R44" s="50"/>
+      <c r="S44" s="50"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="56"/>
-      <c r="J45" s="56"/>
-      <c r="K45" s="56"/>
-      <c r="L45" s="56"/>
-      <c r="M45" s="56"/>
-      <c r="N45" s="56"/>
-      <c r="O45" s="56"/>
-      <c r="P45" s="56"/>
-      <c r="Q45" s="56"/>
-      <c r="R45" s="56"/>
-      <c r="S45" s="56"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="50"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="50"/>
+      <c r="P45" s="50"/>
+      <c r="Q45" s="50"/>
+      <c r="R45" s="50"/>
+      <c r="S45" s="50"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="56"/>
-      <c r="L46" s="56"/>
-      <c r="M46" s="56"/>
-      <c r="N46" s="56"/>
-      <c r="O46" s="56"/>
-      <c r="P46" s="56"/>
-      <c r="Q46" s="56"/>
-      <c r="R46" s="56"/>
-      <c r="S46" s="56"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="50"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="50"/>
+      <c r="P46" s="50"/>
+      <c r="Q46" s="50"/>
+      <c r="R46" s="50"/>
+      <c r="S46" s="50"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B47" s="55"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="56"/>
-      <c r="L47" s="56"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="56"/>
-      <c r="O47" s="56"/>
-      <c r="P47" s="56"/>
-      <c r="Q47" s="56"/>
-      <c r="R47" s="56"/>
-      <c r="S47" s="56"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="50"/>
+      <c r="M47" s="50"/>
+      <c r="N47" s="50"/>
+      <c r="O47" s="50"/>
+      <c r="P47" s="50"/>
+      <c r="Q47" s="50"/>
+      <c r="R47" s="50"/>
+      <c r="S47" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="B2:R3"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B44:C47"/>
+    <mergeCell ref="D44:S47"/>
+    <mergeCell ref="B28:C31"/>
+    <mergeCell ref="D28:S31"/>
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="D32:S35"/>
+    <mergeCell ref="B36:C39"/>
+    <mergeCell ref="D36:S39"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="M11:N11"/>
@@ -3046,30 +3133,6 @@
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="J23:K23"/>
-    <mergeCell ref="B44:C47"/>
-    <mergeCell ref="D44:S47"/>
-    <mergeCell ref="B28:C31"/>
-    <mergeCell ref="D28:S31"/>
-    <mergeCell ref="B32:C35"/>
-    <mergeCell ref="D32:S35"/>
-    <mergeCell ref="B36:C39"/>
-    <mergeCell ref="D36:S39"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="B2:R3"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3092,44 +3155,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="43"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="43"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
     </row>
     <row r="4" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -3193,36 +3256,36 @@
       <c r="D6" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="61"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="70"/>
       <c r="K6" s="34" t="s">
         <v>57</v>
       </c>
       <c r="L6" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="62" t="s">
+      <c r="M6" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="N6" s="62"/>
-      <c r="O6" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="P6" s="61"/>
-      <c r="Q6" s="61" t="s">
-        <v>28</v>
-      </c>
-      <c r="R6" s="63"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="72"/>
     </row>
     <row r="7" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
@@ -3234,36 +3297,36 @@
       <c r="D7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="67"/>
-      <c r="G7" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="64"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="65"/>
       <c r="K7" s="32" t="s">
         <v>61</v>
       </c>
       <c r="L7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M7" s="66" t="s">
+      <c r="M7" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N7" s="66"/>
-      <c r="O7" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R7" s="65"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="66"/>
     </row>
     <row r="8" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="19" t="s">
@@ -3275,36 +3338,36 @@
       <c r="D8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="66"/>
-      <c r="G8" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="64"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="65"/>
       <c r="K8" s="33" t="s">
         <v>64</v>
       </c>
       <c r="L8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="67" t="s">
+      <c r="M8" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="N8" s="67"/>
-      <c r="O8" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R8" s="65"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="66"/>
     </row>
     <row r="9" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
@@ -3316,36 +3379,36 @@
       <c r="D9" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="64"/>
-      <c r="I9" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="64"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="65"/>
       <c r="K9" s="32" t="s">
         <v>67</v>
       </c>
       <c r="L9" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="66" t="s">
+      <c r="M9" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N9" s="66"/>
-      <c r="O9" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R9" s="65"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="66"/>
     </row>
     <row r="10" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="19" t="s">
@@ -3357,36 +3420,36 @@
       <c r="D10" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="66"/>
-      <c r="G10" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="64"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="65"/>
       <c r="K10" s="33" t="s">
         <v>70</v>
       </c>
       <c r="L10" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="67" t="s">
+      <c r="M10" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="N10" s="67"/>
-      <c r="O10" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R10" s="65"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="66"/>
     </row>
     <row r="11" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="19" t="s">
@@ -3398,36 +3461,36 @@
       <c r="D11" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="67" t="s">
+      <c r="E11" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="F11" s="67"/>
-      <c r="G11" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="64"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="65"/>
       <c r="K11" s="32" t="s">
         <v>73</v>
       </c>
       <c r="L11" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="66" t="s">
+      <c r="M11" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N11" s="66"/>
-      <c r="O11" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P11" s="64"/>
-      <c r="Q11" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R11" s="65"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R11" s="66"/>
     </row>
     <row r="12" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="20" t="s">
@@ -3439,36 +3502,36 @@
       <c r="D12" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="66" t="s">
+      <c r="E12" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="66"/>
-      <c r="G12" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="64"/>
-      <c r="I12" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="64"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="65"/>
       <c r="K12" s="33" t="s">
         <v>76</v>
       </c>
       <c r="L12" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M12" s="67" t="s">
+      <c r="M12" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="N12" s="67"/>
-      <c r="O12" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P12" s="64"/>
-      <c r="Q12" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R12" s="65"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="65"/>
+      <c r="Q12" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" s="66"/>
     </row>
     <row r="13" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
@@ -3480,36 +3543,36 @@
       <c r="D13" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="67" t="s">
+      <c r="E13" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="F13" s="67"/>
-      <c r="G13" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J13" s="64"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="65"/>
       <c r="K13" s="32" t="s">
         <v>79</v>
       </c>
       <c r="L13" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="66" t="s">
+      <c r="M13" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="N13" s="66"/>
-      <c r="O13" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P13" s="64"/>
-      <c r="Q13" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R13" s="65"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13" s="66"/>
     </row>
     <row r="14" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="20" t="s">
@@ -3521,36 +3584,36 @@
       <c r="D14" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="66" t="s">
+      <c r="E14" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="F14" s="66"/>
-      <c r="G14" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14" s="64"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="65"/>
       <c r="K14" s="33" t="s">
         <v>93</v>
       </c>
       <c r="L14" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="M14" s="67" t="s">
+      <c r="M14" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="N14" s="67"/>
-      <c r="O14" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="R14" s="65"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="R14" s="66"/>
     </row>
     <row r="15" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="20" t="s">
@@ -3702,334 +3765,357 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="44" t="s">
+      <c r="Q21" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="R21" s="45"/>
+      <c r="R21" s="44"/>
       <c r="T21" s="21"/>
       <c r="U21" s="21"/>
       <c r="V21" s="21"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59">
+      <c r="C23" s="48"/>
+      <c r="D23" s="48">
         <v>7</v>
       </c>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59">
+      <c r="E23" s="48"/>
+      <c r="F23" s="48">
         <v>6</v>
       </c>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59">
+      <c r="G23" s="48"/>
+      <c r="H23" s="48">
         <v>5</v>
       </c>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59">
+      <c r="I23" s="48"/>
+      <c r="J23" s="48">
         <v>4</v>
       </c>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59">
+      <c r="K23" s="48"/>
+      <c r="L23" s="48">
         <v>3</v>
       </c>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59">
+      <c r="M23" s="48"/>
+      <c r="N23" s="48">
         <v>2</v>
       </c>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59">
+      <c r="O23" s="48"/>
+      <c r="P23" s="48">
         <v>1</v>
       </c>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59">
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48">
         <v>0</v>
       </c>
-      <c r="S23" s="59"/>
+      <c r="S23" s="48"/>
     </row>
     <row r="24" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="70" t="s">
+      <c r="C24" s="63"/>
+      <c r="D24" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="70"/>
-      <c r="J24" s="70"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="73" t="s">
-        <v>28</v>
-      </c>
-      <c r="M24" s="73"/>
-      <c r="N24" s="73" t="s">
-        <v>28</v>
-      </c>
-      <c r="O24" s="73"/>
-      <c r="P24" s="73" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q24" s="73"/>
-      <c r="R24" s="70" t="s">
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="64"/>
+      <c r="P24" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" s="64"/>
+      <c r="R24" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="S24" s="70"/>
+      <c r="S24" s="61"/>
     </row>
     <row r="25" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="70"/>
-      <c r="J25" s="70"/>
-      <c r="K25" s="70"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="73"/>
-      <c r="N25" s="73"/>
-      <c r="O25" s="73"/>
-      <c r="P25" s="73"/>
-      <c r="Q25" s="73"/>
-      <c r="R25" s="70"/>
-      <c r="S25" s="70"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="64"/>
+      <c r="Q25" s="64"/>
+      <c r="R25" s="61"/>
+      <c r="S25" s="61"/>
     </row>
     <row r="26" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="73"/>
-      <c r="M26" s="73"/>
-      <c r="N26" s="73"/>
-      <c r="O26" s="73"/>
-      <c r="P26" s="73"/>
-      <c r="Q26" s="73"/>
-      <c r="R26" s="70"/>
-      <c r="S26" s="70"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="64"/>
+      <c r="P26" s="64"/>
+      <c r="Q26" s="64"/>
+      <c r="R26" s="61"/>
+      <c r="S26" s="61"/>
     </row>
     <row r="27" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="70"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="73"/>
-      <c r="M27" s="73"/>
-      <c r="N27" s="73"/>
-      <c r="O27" s="73"/>
-      <c r="P27" s="73"/>
-      <c r="Q27" s="73"/>
-      <c r="R27" s="70"/>
-      <c r="S27" s="70"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="64"/>
+      <c r="P27" s="64"/>
+      <c r="Q27" s="64"/>
+      <c r="R27" s="61"/>
+      <c r="S27" s="61"/>
     </row>
     <row r="28" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="71" t="s">
+      <c r="B28" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="71"/>
-      <c r="D28" s="69" t="s">
+      <c r="C28" s="62"/>
+      <c r="D28" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="69"/>
-      <c r="N28" s="69"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="69"/>
-      <c r="Q28" s="69"/>
-      <c r="R28" s="69"/>
-      <c r="S28" s="69"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="60"/>
+      <c r="R28" s="60"/>
+      <c r="S28" s="60"/>
     </row>
     <row r="29" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="69"/>
-      <c r="M29" s="69"/>
-      <c r="N29" s="69"/>
-      <c r="O29" s="69"/>
-      <c r="P29" s="69"/>
-      <c r="Q29" s="69"/>
-      <c r="R29" s="69"/>
-      <c r="S29" s="69"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
+      <c r="P29" s="60"/>
+      <c r="Q29" s="60"/>
+      <c r="R29" s="60"/>
+      <c r="S29" s="60"/>
     </row>
     <row r="30" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="69"/>
-      <c r="N30" s="69"/>
-      <c r="O30" s="69"/>
-      <c r="P30" s="69"/>
-      <c r="Q30" s="69"/>
-      <c r="R30" s="69"/>
-      <c r="S30" s="69"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="R30" s="60"/>
+      <c r="S30" s="60"/>
     </row>
     <row r="31" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="71"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="69"/>
-      <c r="N31" s="69"/>
-      <c r="O31" s="69"/>
-      <c r="P31" s="69"/>
-      <c r="Q31" s="69"/>
-      <c r="R31" s="69"/>
-      <c r="S31" s="69"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="60"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="60"/>
+      <c r="P31" s="60"/>
+      <c r="Q31" s="60"/>
+      <c r="R31" s="60"/>
+      <c r="S31" s="60"/>
     </row>
     <row r="32" spans="2:22" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="68"/>
-      <c r="D32" s="69" t="s">
+      <c r="C32" s="59"/>
+      <c r="D32" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
-      <c r="N32" s="69"/>
-      <c r="O32" s="69"/>
-      <c r="P32" s="69"/>
-      <c r="Q32" s="69"/>
-      <c r="R32" s="69"/>
-      <c r="S32" s="69"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="60"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="60"/>
+      <c r="R32" s="60"/>
+      <c r="S32" s="60"/>
     </row>
     <row r="33" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="69"/>
-      <c r="N33" s="69"/>
-      <c r="O33" s="69"/>
-      <c r="P33" s="69"/>
-      <c r="Q33" s="69"/>
-      <c r="R33" s="69"/>
-      <c r="S33" s="69"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="60"/>
     </row>
     <row r="34" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="68"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
-      <c r="K34" s="69"/>
-      <c r="L34" s="69"/>
-      <c r="M34" s="69"/>
-      <c r="N34" s="69"/>
-      <c r="O34" s="69"/>
-      <c r="P34" s="69"/>
-      <c r="Q34" s="69"/>
-      <c r="R34" s="69"/>
-      <c r="S34" s="69"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="60"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="60"/>
+      <c r="S34" s="60"/>
     </row>
     <row r="35" spans="2:19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="68"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="69"/>
-      <c r="I35" s="69"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="69"/>
-      <c r="L35" s="69"/>
-      <c r="M35" s="69"/>
-      <c r="N35" s="69"/>
-      <c r="O35" s="69"/>
-      <c r="P35" s="69"/>
-      <c r="Q35" s="69"/>
-      <c r="R35" s="69"/>
-      <c r="S35" s="69"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
+      <c r="L35" s="60"/>
+      <c r="M35" s="60"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B32:C35"/>
-    <mergeCell ref="D32:S35"/>
-    <mergeCell ref="R24:S27"/>
-    <mergeCell ref="B28:C31"/>
-    <mergeCell ref="D28:S31"/>
-    <mergeCell ref="B24:C27"/>
-    <mergeCell ref="D24:K27"/>
-    <mergeCell ref="L24:M27"/>
-    <mergeCell ref="N24:O27"/>
-    <mergeCell ref="P24:Q27"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B2:R3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
     <mergeCell ref="Q13:R13"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="G14:H14"/>
@@ -4042,49 +4128,26 @@
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="M13:N13"/>
     <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="B2:R3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="B32:C35"/>
+    <mergeCell ref="D32:S35"/>
+    <mergeCell ref="R24:S27"/>
+    <mergeCell ref="B28:C31"/>
+    <mergeCell ref="D28:S31"/>
+    <mergeCell ref="B24:C27"/>
+    <mergeCell ref="D24:K27"/>
+    <mergeCell ref="L24:M27"/>
+    <mergeCell ref="N24:O27"/>
+    <mergeCell ref="P24:Q27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>